<commit_message>
test for paper upd.
</commit_message>
<xml_diff>
--- a/migforecasting/social conflicts/test for paper.xlsx
+++ b/migforecasting/social conflicts/test for paper.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>train (R2)</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t xml:space="preserve"> (conflict-21, top300, formodel-2).csv)</t>
+  </si>
+  <si>
+    <t>train (MAE)</t>
+  </si>
+  <si>
+    <t>test (MAE)</t>
   </si>
 </sst>
 </file>
@@ -464,23 +470,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:J57"/>
+  <dimension ref="C1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="12.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
@@ -489,16 +507,30 @@
         <v>5</v>
       </c>
       <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="1"/>
+      <c r="S2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="1"/>
+    </row>
+    <row r="3" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -513,8 +545,22 @@
       <c r="J4" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N4" s="2"/>
+      <c r="O4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -533,8 +579,26 @@
       <c r="J5" s="3">
         <v>0.64275982298876144</v>
       </c>
-    </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.11629864236609461</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.31224638203978711</v>
+      </c>
+      <c r="S5" s="2">
+        <v>1</v>
+      </c>
+      <c r="T5" s="3">
+        <v>8.1769613043519596E-2</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0.2185752247090387</v>
+      </c>
+    </row>
+    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -555,8 +619,28 @@
       <c r="J6" s="3">
         <v>0.629469090151622</v>
       </c>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N6" s="2">
+        <f>N5+1</f>
+        <v>2</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.1168169117142514</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0.31273421380824667</v>
+      </c>
+      <c r="S6" s="2">
+        <f>S5+1</f>
+        <v>2</v>
+      </c>
+      <c r="T6" s="3">
+        <v>8.2015583435031403E-2</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0.228059986916406</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -577,8 +661,28 @@
       <c r="J7" s="3">
         <v>0.66944149512898354</v>
       </c>
-    </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N7" s="2">
+        <f t="shared" ref="N7:N54" si="2">N6+1</f>
+        <v>3</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0.1179096055996649</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0.29563574077515559</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" ref="S7:S54" si="3">S6+1</f>
+        <v>3</v>
+      </c>
+      <c r="T7" s="3">
+        <v>8.2242710734438632E-2</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0.2149826377335019</v>
+      </c>
+    </row>
+    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -599,8 +703,28 @@
       <c r="J8" s="3">
         <v>0.68654267551945458</v>
       </c>
-    </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0.1172464566941234</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0.30646210688982789</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="T8" s="3">
+        <v>8.1549176794793454E-2</v>
+      </c>
+      <c r="U8" s="3">
+        <v>0.22654039805285689</v>
+      </c>
+    </row>
+    <row r="9" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -621,8 +745,28 @@
       <c r="J9" s="3">
         <v>0.66641103683849501</v>
       </c>
-    </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0.11815620674558699</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0.30697978105111479</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="T9" s="3">
+        <v>8.1536264136596287E-2</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0.22159406681404359</v>
+      </c>
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -643,8 +787,28 @@
       <c r="J10" s="3">
         <v>0.6532349561766656</v>
       </c>
-    </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0.1169240315092835</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0.30980523001355198</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="T10" s="3">
+        <v>8.1823070141145773E-2</v>
+      </c>
+      <c r="U10" s="3">
+        <v>0.22855806711828469</v>
+      </c>
+    </row>
+    <row r="11" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -665,8 +829,28 @@
       <c r="J11" s="3">
         <v>0.65712144013742768</v>
       </c>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0.1162986700492049</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.32155039855673279</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="T11" s="3">
+        <v>8.1705863850174379E-2</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0.21721269051565181</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -687,8 +871,28 @@
       <c r="J12" s="3">
         <v>0.62811490133172454</v>
       </c>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0.11776354951009541</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0.31911434022278012</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="T12" s="3">
+        <v>8.2664068657790857E-2</v>
+      </c>
+      <c r="U12" s="3">
+        <v>0.21594411354817489</v>
+      </c>
+    </row>
+    <row r="13" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -709,8 +913,28 @@
       <c r="J13" s="3">
         <v>0.64387148219708357</v>
       </c>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0.1156787760033966</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0.31468487648743998</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="T13" s="3">
+        <v>8.2246020605867914E-2</v>
+      </c>
+      <c r="U13" s="3">
+        <v>0.22114865492312391</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -731,8 +955,28 @@
       <c r="J14" s="3">
         <v>0.67642291136019894</v>
       </c>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0.1178000635324878</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0.30004516193868969</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="T14" s="3">
+        <v>8.2762723030266369E-2</v>
+      </c>
+      <c r="U14" s="3">
+        <v>0.22181721225600909</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -753,8 +997,28 @@
       <c r="J15" s="3">
         <v>0.66143118076609753</v>
       </c>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0.1171383818317885</v>
+      </c>
+      <c r="P15" s="3">
+        <v>0.30811545296515908</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="T15" s="3">
+        <v>8.3102819747522774E-2</v>
+      </c>
+      <c r="U15" s="3">
+        <v>0.2112029915425882</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -775,8 +1039,28 @@
       <c r="J16" s="3">
         <v>0.67018187713441957</v>
       </c>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0.1171186160910848</v>
+      </c>
+      <c r="P16" s="3">
+        <v>0.31103563353080099</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="T16" s="3">
+        <v>8.2339487334254086E-2</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0.2260417239367816</v>
+      </c>
+    </row>
+    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -797,8 +1081,28 @@
       <c r="J17" s="3">
         <v>0.62043554495858433</v>
       </c>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O17" s="3">
+        <v>0.1171742453010904</v>
+      </c>
+      <c r="P17" s="3">
+        <v>0.31140957698377753</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="T17" s="3">
+        <v>8.1596317207806829E-2</v>
+      </c>
+      <c r="U17" s="3">
+        <v>0.23112952553723701</v>
+      </c>
+    </row>
+    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -819,8 +1123,28 @@
       <c r="J18" s="3">
         <v>0.65092072927518974</v>
       </c>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0.1164586784263299</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0.30973552394199477</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="T18" s="3">
+        <v>8.2632752639061433E-2</v>
+      </c>
+      <c r="U18" s="3">
+        <v>0.21940649077523819</v>
+      </c>
+    </row>
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -841,8 +1165,28 @@
       <c r="J19" s="3">
         <v>0.63727055500260632</v>
       </c>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O19" s="3">
+        <v>0.1177906235918996</v>
+      </c>
+      <c r="P19" s="3">
+        <v>0.30600599996569089</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="T19" s="3">
+        <v>8.1650285344827836E-2</v>
+      </c>
+      <c r="U19" s="3">
+        <v>0.22222848595890529</v>
+      </c>
+    </row>
+    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -863,8 +1207,28 @@
       <c r="J20" s="3">
         <v>0.67338195669841994</v>
       </c>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O20" s="3">
+        <v>0.11747927165115141</v>
+      </c>
+      <c r="P20" s="3">
+        <v>0.31312975008720212</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="T20" s="3">
+        <v>8.2300244262586322E-2</v>
+      </c>
+      <c r="U20" s="3">
+        <v>0.2131942670611168</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -885,8 +1249,28 @@
       <c r="J21" s="3">
         <v>0.6026267589083667</v>
       </c>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0.1170660597063146</v>
+      </c>
+      <c r="P21" s="3">
+        <v>0.31892808825715768</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="T21" s="3">
+        <v>8.2010057078785031E-2</v>
+      </c>
+      <c r="U21" s="3">
+        <v>0.22226383573189001</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -907,8 +1291,28 @@
       <c r="J22" s="3">
         <v>0.61387782259502877</v>
       </c>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0.1190566414304584</v>
+      </c>
+      <c r="P22" s="3">
+        <v>0.29201141261772301</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="T22" s="3">
+        <v>8.2465725949413093E-2</v>
+      </c>
+      <c r="U22" s="3">
+        <v>0.22775780337315041</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -929,8 +1333,28 @@
       <c r="J23" s="3">
         <v>0.67092602974066218</v>
       </c>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O23" s="3">
+        <v>0.1170426397950606</v>
+      </c>
+      <c r="P23" s="3">
+        <v>0.31211045796856152</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="T23" s="3">
+        <v>8.1284535638414881E-2</v>
+      </c>
+      <c r="U23" s="3">
+        <v>0.2249461185399371</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -951,8 +1375,28 @@
       <c r="J24" s="3">
         <v>0.64708949151819772</v>
       </c>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O24" s="3">
+        <v>0.1170295318423671</v>
+      </c>
+      <c r="P24" s="3">
+        <v>0.30995721028871059</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="T24" s="3">
+        <v>8.2756239960734349E-2</v>
+      </c>
+      <c r="U24" s="3">
+        <v>0.2251606878609029</v>
+      </c>
+    </row>
+    <row r="25" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -973,8 +1417,28 @@
       <c r="J25" s="3">
         <v>0.62155754559636966</v>
       </c>
-    </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O25" s="3">
+        <v>0.1159687288999377</v>
+      </c>
+      <c r="P25" s="3">
+        <v>0.3253760936579731</v>
+      </c>
+      <c r="S25" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="T25" s="3">
+        <v>8.2789932906881553E-2</v>
+      </c>
+      <c r="U25" s="3">
+        <v>0.22213151164887629</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -995,8 +1459,28 @@
       <c r="J26" s="3">
         <v>0.65686887250701631</v>
       </c>
-    </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O26" s="3">
+        <v>0.1188156322728026</v>
+      </c>
+      <c r="P26" s="3">
+        <v>0.30442573730136491</v>
+      </c>
+      <c r="S26" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="T26" s="3">
+        <v>8.1020708579676914E-2</v>
+      </c>
+      <c r="U26" s="3">
+        <v>0.21822296232072161</v>
+      </c>
+    </row>
+    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1017,8 +1501,28 @@
       <c r="J27" s="3">
         <v>0.65923397279026807</v>
       </c>
-    </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O27" s="3">
+        <v>0.11645404150536651</v>
+      </c>
+      <c r="P27" s="3">
+        <v>0.31879587372270279</v>
+      </c>
+      <c r="S27" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="T27" s="3">
+        <v>8.1844616988188068E-2</v>
+      </c>
+      <c r="U27" s="3">
+        <v>0.22593443927629869</v>
+      </c>
+    </row>
+    <row r="28" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1039,8 +1543,28 @@
       <c r="J28" s="3">
         <v>0.61945516198522554</v>
       </c>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O28" s="3">
+        <v>0.1157431253931244</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0.31943845407734389</v>
+      </c>
+      <c r="S28" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="T28" s="3">
+        <v>8.2173262857609272E-2</v>
+      </c>
+      <c r="U28" s="3">
+        <v>0.21537597522765939</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1061,8 +1585,28 @@
       <c r="J29" s="3">
         <v>0.62156571497581037</v>
       </c>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0.11867626165435349</v>
+      </c>
+      <c r="P29" s="3">
+        <v>0.3004675508345675</v>
+      </c>
+      <c r="S29" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="T29" s="3">
+        <v>8.3103598191252098E-2</v>
+      </c>
+      <c r="U29" s="3">
+        <v>0.21896354956737649</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1083,8 +1627,28 @@
       <c r="J30" s="3">
         <v>0.66045691000948448</v>
       </c>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O30" s="3">
+        <v>0.1169732797623813</v>
+      </c>
+      <c r="P30" s="3">
+        <v>0.3032128295097809</v>
+      </c>
+      <c r="S30" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="T30" s="3">
+        <v>8.3415777895986545E-2</v>
+      </c>
+      <c r="U30" s="3">
+        <v>0.21674506623377729</v>
+      </c>
+    </row>
+    <row r="31" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1105,8 +1669,28 @@
       <c r="J31" s="3">
         <v>0.63145951918685972</v>
       </c>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O31" s="3">
+        <v>0.1163453991392718</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0.32424540470377</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="T31" s="3">
+        <v>8.199141602551098E-2</v>
+      </c>
+      <c r="U31" s="3">
+        <v>0.22104538512261029</v>
+      </c>
+    </row>
+    <row r="32" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1127,8 +1711,28 @@
       <c r="J32" s="3">
         <v>0.64038552491857614</v>
       </c>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O32" s="3">
+        <v>0.11644616566050631</v>
+      </c>
+      <c r="P32" s="3">
+        <v>0.31759852383906773</v>
+      </c>
+      <c r="S32" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="T32" s="3">
+        <v>8.1993014509199463E-2</v>
+      </c>
+      <c r="U32" s="3">
+        <v>0.22662824984082541</v>
+      </c>
+    </row>
+    <row r="33" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1149,8 +1753,28 @@
       <c r="J33" s="3">
         <v>0.65931224638203723</v>
       </c>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O33" s="3">
+        <v>0.11672428402742439</v>
+      </c>
+      <c r="P33" s="3">
+        <v>0.31902442548075549</v>
+      </c>
+      <c r="S33" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="T33" s="3">
+        <v>8.2309728202983323E-2</v>
+      </c>
+      <c r="U33" s="3">
+        <v>0.22590961366287871</v>
+      </c>
+    </row>
+    <row r="34" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1171,8 +1795,28 @@
       <c r="J34" s="3">
         <v>0.67417057297540284</v>
       </c>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O34" s="3">
+        <v>0.1169542614656538</v>
+      </c>
+      <c r="P34" s="3">
+        <v>0.32529631093429251</v>
+      </c>
+      <c r="S34" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="T34" s="3">
+        <v>8.1605759551974022E-2</v>
+      </c>
+      <c r="U34" s="3">
+        <v>0.22718560267952981</v>
+      </c>
+    </row>
+    <row r="35" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1193,8 +1837,28 @@
       <c r="J35" s="3">
         <v>0.67312707425646479</v>
       </c>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O35" s="3">
+        <v>0.1171298554338379</v>
+      </c>
+      <c r="P35" s="3">
+        <v>0.30882175983954802</v>
+      </c>
+      <c r="S35" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="T35" s="3">
+        <v>8.0857996013291869E-2</v>
+      </c>
+      <c r="U35" s="3">
+        <v>0.23442192452121891</v>
+      </c>
+    </row>
+    <row r="36" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1215,8 +1879,28 @@
       <c r="J36" s="3">
         <v>0.68213548431407811</v>
       </c>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O36" s="3">
+        <v>0.11464950412351831</v>
+      </c>
+      <c r="P36" s="3">
+        <v>0.31775017191690352</v>
+      </c>
+      <c r="S36" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="T36" s="3">
+        <v>8.268426659852357E-2</v>
+      </c>
+      <c r="U36" s="3">
+        <v>0.214568109380808</v>
+      </c>
+    </row>
+    <row r="37" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1237,8 +1921,28 @@
       <c r="J37" s="3">
         <v>0.66254879724570159</v>
       </c>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O37" s="3">
+        <v>0.1192575516029472</v>
+      </c>
+      <c r="P37" s="3">
+        <v>0.30416485167056451</v>
+      </c>
+      <c r="S37" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="T37" s="3">
+        <v>8.251939102818831E-2</v>
+      </c>
+      <c r="U37" s="3">
+        <v>0.22075695663214909</v>
+      </c>
+    </row>
+    <row r="38" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1259,8 +1963,28 @@
       <c r="J38" s="3">
         <v>0.62595058311489304</v>
       </c>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O38" s="3">
+        <v>0.116326574624316</v>
+      </c>
+      <c r="P38" s="3">
+        <v>0.31101830390379742</v>
+      </c>
+      <c r="S38" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="T38" s="3">
+        <v>8.2179918254379064E-2</v>
+      </c>
+      <c r="U38" s="3">
+        <v>0.22428725388674131</v>
+      </c>
+    </row>
+    <row r="39" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1281,8 +2005,28 @@
       <c r="J39" s="3">
         <v>0.66168153920180028</v>
       </c>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O39" s="3">
+        <v>0.11657180545628169</v>
+      </c>
+      <c r="P39" s="3">
+        <v>0.32267682431196071</v>
+      </c>
+      <c r="S39" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="T39" s="3">
+        <v>8.434088398931025E-2</v>
+      </c>
+      <c r="U39" s="3">
+        <v>0.2074504515956096</v>
+      </c>
+    </row>
+    <row r="40" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1303,8 +2047,28 @@
       <c r="J40" s="3">
         <v>0.65877402667637974</v>
       </c>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O40" s="3">
+        <v>0.1175172251952756</v>
+      </c>
+      <c r="P40" s="3">
+        <v>0.29687029675893889</v>
+      </c>
+      <c r="S40" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="T40" s="3">
+        <v>8.1053474524131197E-2</v>
+      </c>
+      <c r="U40" s="3">
+        <v>0.2234413775313043</v>
+      </c>
+    </row>
+    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1325,8 +2089,28 @@
       <c r="J41" s="3">
         <v>0.60822670067763585</v>
       </c>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O41" s="3">
+        <v>0.1163592268528314</v>
+      </c>
+      <c r="P41" s="3">
+        <v>0.33429847081729869</v>
+      </c>
+      <c r="S41" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="T41" s="3">
+        <v>8.2970175312972821E-2</v>
+      </c>
+      <c r="U41" s="3">
+        <v>0.21663735395507289</v>
+      </c>
+    </row>
+    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1347,8 +2131,28 @@
       <c r="J42" s="3">
         <v>0.67173315570091452</v>
       </c>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O42" s="3">
+        <v>0.1171025183624865</v>
+      </c>
+      <c r="P42" s="3">
+        <v>0.30969333488200551</v>
+      </c>
+      <c r="S42" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="T42" s="3">
+        <v>8.2391958007001886E-2</v>
+      </c>
+      <c r="U42" s="3">
+        <v>0.2213559784908905</v>
+      </c>
+    </row>
+    <row r="43" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1369,8 +2173,28 @@
       <c r="J43" s="3">
         <v>0.62366652977891113</v>
       </c>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O43" s="3">
+        <v>0.1160097829524077</v>
+      </c>
+      <c r="P43" s="3">
+        <v>0.31411067341506499</v>
+      </c>
+      <c r="S43" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="T43" s="3">
+        <v>8.22429721964546E-2</v>
+      </c>
+      <c r="U43" s="3">
+        <v>0.22404168224471041</v>
+      </c>
+    </row>
+    <row r="44" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1391,8 +2215,28 @@
       <c r="J44" s="3">
         <v>0.66709565694910156</v>
       </c>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O44" s="3">
+        <v>0.1169842007493667</v>
+      </c>
+      <c r="P44" s="3">
+        <v>0.3195361200902328</v>
+      </c>
+      <c r="S44" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="T44" s="3">
+        <v>8.1921480878560951E-2</v>
+      </c>
+      <c r="U44" s="3">
+        <v>0.22349437843421341</v>
+      </c>
+    </row>
+    <row r="45" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1413,8 +2257,28 @@
       <c r="J45" s="3">
         <v>0.65934202866357861</v>
       </c>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O45" s="3">
+        <v>0.1156723396802683</v>
+      </c>
+      <c r="P45" s="3">
+        <v>0.32980129419433779</v>
+      </c>
+      <c r="S45" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="T45" s="3">
+        <v>8.265138180769839E-2</v>
+      </c>
+      <c r="U45" s="3">
+        <v>0.2185944437724423</v>
+      </c>
+    </row>
+    <row r="46" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1435,8 +2299,28 @@
       <c r="J46" s="3">
         <v>0.66645550777495477</v>
       </c>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O46" s="3">
+        <v>0.1192893179719352</v>
+      </c>
+      <c r="P46" s="3">
+        <v>0.30232087969819471</v>
+      </c>
+      <c r="S46" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="T46" s="3">
+        <v>8.1484548138303636E-2</v>
+      </c>
+      <c r="U46" s="3">
+        <v>0.2207778386553034</v>
+      </c>
+    </row>
+    <row r="47" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1457,8 +2341,28 @@
       <c r="J47" s="3">
         <v>0.6887499196782334</v>
       </c>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O47" s="3">
+        <v>0.1148393825765807</v>
+      </c>
+      <c r="P47" s="3">
+        <v>0.32812220282649351</v>
+      </c>
+      <c r="S47" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="T47" s="3">
+        <v>8.2216713090806512E-2</v>
+      </c>
+      <c r="U47" s="3">
+        <v>0.2176719762422053</v>
+      </c>
+    </row>
+    <row r="48" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1479,8 +2383,28 @@
       <c r="J48" s="3">
         <v>0.67400105812749556</v>
       </c>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O48" s="3">
+        <v>0.1183066921327932</v>
+      </c>
+      <c r="P48" s="3">
+        <v>0.31167400605268719</v>
+      </c>
+      <c r="S48" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="T48" s="3">
+        <v>8.1229551364922783E-2</v>
+      </c>
+      <c r="U48" s="3">
+        <v>0.22558488513671829</v>
+      </c>
+    </row>
+    <row r="49" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1501,8 +2425,28 @@
       <c r="J49" s="3">
         <v>0.67184601578768866</v>
       </c>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O49" s="3">
+        <v>0.1181313888372665</v>
+      </c>
+      <c r="P49" s="3">
+        <v>0.2993634376661844</v>
+      </c>
+      <c r="S49" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="T49" s="3">
+        <v>8.1252399579726312E-2</v>
+      </c>
+      <c r="U49" s="3">
+        <v>0.22627686644551931</v>
+      </c>
+    </row>
+    <row r="50" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1523,8 +2467,28 @@
       <c r="J50" s="3">
         <v>0.6561462463634381</v>
       </c>
-    </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O50" s="3">
+        <v>0.11526373697328469</v>
+      </c>
+      <c r="P50" s="3">
+        <v>0.32834649138557082</v>
+      </c>
+      <c r="S50" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="T50" s="3">
+        <v>8.1913761806771665E-2</v>
+      </c>
+      <c r="U50" s="3">
+        <v>0.22526419522709509</v>
+      </c>
+    </row>
+    <row r="51" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1545,8 +2509,28 @@
       <c r="J51" s="3">
         <v>0.62565473218451251</v>
       </c>
-    </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O51" s="3">
+        <v>0.1167540156878106</v>
+      </c>
+      <c r="P51" s="3">
+        <v>0.31376120183153111</v>
+      </c>
+      <c r="S51" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="T51" s="3">
+        <v>8.2386580208719126E-2</v>
+      </c>
+      <c r="U51" s="3">
+        <v>0.2183309121651047</v>
+      </c>
+    </row>
+    <row r="52" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1567,8 +2551,28 @@
       <c r="J52" s="3">
         <v>0.67470635833973236</v>
       </c>
-    </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O52" s="3">
+        <v>0.115755029130523</v>
+      </c>
+      <c r="P52" s="3">
+        <v>0.316101255139209</v>
+      </c>
+      <c r="S52" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="T52" s="3">
+        <v>8.2620642193867777E-2</v>
+      </c>
+      <c r="U52" s="3">
+        <v>0.2183574957645468</v>
+      </c>
+    </row>
+    <row r="53" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1589,8 +2593,28 @@
       <c r="J53" s="3">
         <v>0.67214288983268911</v>
       </c>
-    </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O53" s="3">
+        <v>0.1179774430612817</v>
+      </c>
+      <c r="P53" s="3">
+        <v>0.31719008723074549</v>
+      </c>
+      <c r="S53" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="T53" s="3">
+        <v>8.317294504866625E-2</v>
+      </c>
+      <c r="U53" s="3">
+        <v>0.2208504624832697</v>
+      </c>
+    </row>
+    <row r="54" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1611,8 +2635,28 @@
       <c r="J54" s="3">
         <v>0.66955852923017856</v>
       </c>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O54" s="3">
+        <v>0.11672725996177399</v>
+      </c>
+      <c r="P54" s="3">
+        <v>0.31912823714411509</v>
+      </c>
+      <c r="S54" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="T54" s="3">
+        <v>8.2903110305879796E-2</v>
+      </c>
+      <c r="U54" s="3">
+        <v>0.22718864352021659</v>
+      </c>
+    </row>
+    <row r="56" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -1635,8 +2679,30 @@
         <f>AVERAGE(J5:J54)</f>
         <v>0.65279081267306827</v>
       </c>
-    </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="N56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O56" s="3">
+        <f>AVERAGE(O5:O54)</f>
+        <v>0.11699947269078689</v>
+      </c>
+      <c r="P56" s="3">
+        <f>AVERAGE(P5:P54)</f>
+        <v>0.31308656886454217</v>
+      </c>
+      <c r="S56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T56" s="3">
+        <f>AVERAGE(T5:T54)</f>
+        <v>8.2193910513009422E-2</v>
+      </c>
+      <c r="U56" s="3">
+        <f>AVERAGE(U5:U54)</f>
+        <v>0.22170521049141068</v>
+      </c>
+    </row>
+    <row r="57" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -1658,6 +2724,28 @@
       <c r="J57" s="3">
         <f>_xlfn.STDEV.S(J5:J54)</f>
         <v>2.2180145922211052E-2</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O57" s="3">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
+        <v>1.0573885580347465E-3</v>
+      </c>
+      <c r="P57" s="3">
+        <f>_xlfn.STDEV.S(P5:P54)</f>
+        <v>9.2969639757002707E-3</v>
+      </c>
+      <c r="S57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T57" s="3">
+        <f>_xlfn.STDEV.S(T5:T54)</f>
+        <v>6.7919170904217252E-4</v>
+      </c>
+      <c r="U57" s="3">
+        <f>_xlfn.STDEV.S(U5:U54)</f>
+        <v>5.2278534035366938E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test for paper (age struct)
</commit_message>
<xml_diff>
--- a/migforecasting/social conflicts/test for paper.xlsx
+++ b/migforecasting/social conflicts/test for paper.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="error" sheetId="1" r:id="rId1"/>
-    <sheet name="signif" sheetId="2" r:id="rId2"/>
+    <sheet name="error (soc-eco)" sheetId="1" r:id="rId1"/>
+    <sheet name="error (dem)" sheetId="3" r:id="rId2"/>
+    <sheet name="signif" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>train (R2)</t>
   </si>
@@ -104,13 +105,151 @@
   </si>
   <si>
     <t>test (MAE)</t>
+  </si>
+  <si>
+    <t>0-4</t>
+  </si>
+  <si>
+    <t>5-9</t>
+  </si>
+  <si>
+    <t>10-14</t>
+  </si>
+  <si>
+    <t>15-19</t>
+  </si>
+  <si>
+    <t>20-24</t>
+  </si>
+  <si>
+    <t>25-29</t>
+  </si>
+  <si>
+    <t>30-34</t>
+  </si>
+  <si>
+    <t>35-39</t>
+  </si>
+  <si>
+    <t>40-44</t>
+  </si>
+  <si>
+    <t>45-49</t>
+  </si>
+  <si>
+    <t>50-54</t>
+  </si>
+  <si>
+    <t>55-59</t>
+  </si>
+  <si>
+    <t>60-64</t>
+  </si>
+  <si>
+    <t>65-69</t>
+  </si>
+  <si>
+    <t>(avgage-superdataset-24-alltime-clust (IQR)-normbysoul-f</t>
+  </si>
+  <si>
+    <t>avgage</t>
+  </si>
+  <si>
+    <t>(agerow-superdataset-24-alltime-clust (IQR)-normbysoul-f</t>
+  </si>
+  <si>
+    <t>0-4_male</t>
+  </si>
+  <si>
+    <t>5-9_male</t>
+  </si>
+  <si>
+    <t>10-14_male</t>
+  </si>
+  <si>
+    <t>15-19_male</t>
+  </si>
+  <si>
+    <t>20-24_male</t>
+  </si>
+  <si>
+    <t>25-29_male</t>
+  </si>
+  <si>
+    <t>30-34_male</t>
+  </si>
+  <si>
+    <t>35-39_male</t>
+  </si>
+  <si>
+    <t>40-44_male</t>
+  </si>
+  <si>
+    <t>45-49_male</t>
+  </si>
+  <si>
+    <t>50-54_male</t>
+  </si>
+  <si>
+    <t>55-59_male</t>
+  </si>
+  <si>
+    <t>60-64_male</t>
+  </si>
+  <si>
+    <t>65-69_male</t>
+  </si>
+  <si>
+    <t>0-4_female</t>
+  </si>
+  <si>
+    <t>5-9_female</t>
+  </si>
+  <si>
+    <t>10-14_female</t>
+  </si>
+  <si>
+    <t>15-19_female</t>
+  </si>
+  <si>
+    <t>20-24_female</t>
+  </si>
+  <si>
+    <t>25-29_female</t>
+  </si>
+  <si>
+    <t>30-34_female</t>
+  </si>
+  <si>
+    <t>35-39_female</t>
+  </si>
+  <si>
+    <t>40-44_female</t>
+  </si>
+  <si>
+    <t>45-49_female</t>
+  </si>
+  <si>
+    <t>50-54_female</t>
+  </si>
+  <si>
+    <t>55-59_female</t>
+  </si>
+  <si>
+    <t>60-64_female</t>
+  </si>
+  <si>
+    <t>65-69_female</t>
+  </si>
+  <si>
+    <t>agerow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +290,11 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -172,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -189,6 +333,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2756,10 +2903,1214 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:D20"/>
+  <dimension ref="D2:L58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.89710417727868963</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.26818729527531049</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.90729947776996445</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.30138002696576222</v>
+      </c>
+    </row>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <f>D6+1</f>
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.89844526287566817</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.2261206792417039</v>
+      </c>
+      <c r="J7" s="2">
+        <f>J6+1</f>
+        <v>2</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.90453732905272644</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.33605610666232788</v>
+      </c>
+    </row>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <f t="shared" ref="D8:D55" si="0">D7+1</f>
+        <v>3</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.89833842305614253</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.26463127992501662</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" ref="J8:J55" si="1">J7+1</f>
+        <v>3</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.90634310003394225</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.31550163596450448</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.89958574663382662</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.2745112093809744</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.90496776123943767</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.34040323335747003</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.89793467778235114</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.28398710471662753</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.90627679672742345</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.2856393139030704</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.89771673934811913</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.27296211706149998</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.90482907765804699</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.32350897458847039</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.89919241917540083</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.26233267711727343</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.90711654164017819</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.31172778499274828</v>
+      </c>
+    </row>
+    <row r="13" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.89624864781101443</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.27324999616583151</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.9070408177586653</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.36464165434328472</v>
+      </c>
+    </row>
+    <row r="14" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.89940330018337533</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.25865140992048891</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0.90680025960378041</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0.31966052725589239</v>
+      </c>
+    </row>
+    <row r="15" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.89866033151968883</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.2351722376086591</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.90590947691463908</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0.35906007628160869</v>
+      </c>
+    </row>
+    <row r="16" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.89905264479029645</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.30668965003446402</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.90594593788745892</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0.31808632689186728</v>
+      </c>
+    </row>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.89978665441388461</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.25714672682626649</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.90484188397091125</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0.30758642450531831</v>
+      </c>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.89865844657109417</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.24947929999899959</v>
+      </c>
+      <c r="J18" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.90596487131354675</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.32070142630575699</v>
+      </c>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.89799217174016066</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.31364417652716903</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0.9069682665093971</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.30549426965808041</v>
+      </c>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.89389352546193801</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.29548887863172663</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.90891542634736688</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.28729591536322102</v>
+      </c>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.89844342298667401</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0.29904476936040209</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.90514206201650027</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0.32283470611445708</v>
+      </c>
+    </row>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.8945468918617312</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.30961312774935412</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.90354728790772931</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0.34791311662321012</v>
+      </c>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.89661243904052168</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.29301145323821459</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0.90626839177978047</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.27819203103218942</v>
+      </c>
+    </row>
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.89704969500031972</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.30596824557868019</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0.90677026900242663</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0.33051649428899599</v>
+      </c>
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.89611185474293498</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.24968965398616469</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.90774746551355912</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0.31334375349141319</v>
+      </c>
+    </row>
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.89721925342926112</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.30089253148125578</v>
+      </c>
+      <c r="J26" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.90547632321899174</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0.32047435147645048</v>
+      </c>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.89640534499323843</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.28898947601744851</v>
+      </c>
+      <c r="J27" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0.90521034191213445</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0.35566017575288672</v>
+      </c>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.8992682546853128</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.26382343512627221</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.90292739820445433</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0.33514263685159013</v>
+      </c>
+    </row>
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.89815425245495906</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.30244915485993162</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0.90772126145404974</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0.30821721905365829</v>
+      </c>
+    </row>
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.89928524223062412</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.28704568827427568</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0.904697421130913</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0.34914379939291379</v>
+      </c>
+    </row>
+    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.89804849017084609</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.29279654586376519</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0.90718240503389791</v>
+      </c>
+      <c r="L31" s="3">
+        <v>0.31181950741017489</v>
+      </c>
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.89617613229107296</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0.27841261887597002</v>
+      </c>
+      <c r="J32" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="K32" s="3">
+        <v>0.90732264106647842</v>
+      </c>
+      <c r="L32" s="3">
+        <v>0.3091955641571783</v>
+      </c>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.89819561170927487</v>
+      </c>
+      <c r="F33" s="3">
+        <v>0.27460237732291892</v>
+      </c>
+      <c r="J33" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="K33" s="3">
+        <v>0.90276746056687007</v>
+      </c>
+      <c r="L33" s="3">
+        <v>0.33298812020121588</v>
+      </c>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.89862453096985084</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0.2235630712993191</v>
+      </c>
+      <c r="J34" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="K34" s="3">
+        <v>0.90660429609040316</v>
+      </c>
+      <c r="L34" s="3">
+        <v>0.30580620990159341</v>
+      </c>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.89830333750867619</v>
+      </c>
+      <c r="F35" s="3">
+        <v>0.25270065629008892</v>
+      </c>
+      <c r="J35" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="K35" s="3">
+        <v>0.907372243852134</v>
+      </c>
+      <c r="L35" s="3">
+        <v>0.33211367010758341</v>
+      </c>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.89615609958482612</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0.25803149899587258</v>
+      </c>
+      <c r="J36" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="K36" s="3">
+        <v>0.90614418710388023</v>
+      </c>
+      <c r="L36" s="3">
+        <v>0.29615609697219258</v>
+      </c>
+    </row>
+    <row r="37" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.89655359841142035</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0.26976277615200661</v>
+      </c>
+      <c r="J37" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0.90682318086615654</v>
+      </c>
+      <c r="L37" s="3">
+        <v>0.29381406280476791</v>
+      </c>
+    </row>
+    <row r="38" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0.89687879949098082</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0.26570226191517909</v>
+      </c>
+      <c r="J38" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0.90774080246328848</v>
+      </c>
+      <c r="L38" s="3">
+        <v>0.29108931258119852</v>
+      </c>
+    </row>
+    <row r="39" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.89791636842458056</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.2707900903834477</v>
+      </c>
+      <c r="J39" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0.90517543957709057</v>
+      </c>
+      <c r="L39" s="3">
+        <v>0.35666862901144109</v>
+      </c>
+    </row>
+    <row r="40" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.89866214526602051</v>
+      </c>
+      <c r="F40" s="3">
+        <v>0.27287301168532668</v>
+      </c>
+      <c r="J40" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="K40" s="3">
+        <v>0.90677225972663833</v>
+      </c>
+      <c r="L40" s="3">
+        <v>0.34281492183782147</v>
+      </c>
+    </row>
+    <row r="41" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.89711451066997516</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.30263906726792372</v>
+      </c>
+      <c r="J41" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="K41" s="3">
+        <v>0.90507710767794458</v>
+      </c>
+      <c r="L41" s="3">
+        <v>0.31052113871149611</v>
+      </c>
+    </row>
+    <row r="42" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.89735764765705883</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.27080073259838822</v>
+      </c>
+      <c r="J42" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0.90457541543937847</v>
+      </c>
+      <c r="L42" s="3">
+        <v>0.35907823165696667</v>
+      </c>
+    </row>
+    <row r="43" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0.89692826001478121</v>
+      </c>
+      <c r="F43" s="3">
+        <v>0.30235905765278381</v>
+      </c>
+      <c r="J43" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0.90609319503778751</v>
+      </c>
+      <c r="L43" s="3">
+        <v>0.31675399132070903</v>
+      </c>
+    </row>
+    <row r="44" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0.89809930626562895</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0.26999799855731288</v>
+      </c>
+      <c r="J44" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0.90780783970153789</v>
+      </c>
+      <c r="L44" s="3">
+        <v>0.32634483448152529</v>
+      </c>
+    </row>
+    <row r="45" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0.89868060867510258</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.2955355754351664</v>
+      </c>
+      <c r="J45" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0.90882122626077899</v>
+      </c>
+      <c r="L45" s="3">
+        <v>0.32048463042837422</v>
+      </c>
+    </row>
+    <row r="46" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0.8972407049592771</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0.29630157871071189</v>
+      </c>
+      <c r="J46" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="K46" s="3">
+        <v>0.90460452488302978</v>
+      </c>
+      <c r="L46" s="3">
+        <v>0.31959327377859481</v>
+      </c>
+    </row>
+    <row r="47" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0.89636894537575762</v>
+      </c>
+      <c r="F47" s="3">
+        <v>0.28803455368732878</v>
+      </c>
+      <c r="J47" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="K47" s="3">
+        <v>0.90484529705829164</v>
+      </c>
+      <c r="L47" s="3">
+        <v>0.34590476000107417</v>
+      </c>
+    </row>
+    <row r="48" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0.89741687384364055</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0.27738225896947333</v>
+      </c>
+      <c r="J48" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0.90604040458777069</v>
+      </c>
+      <c r="L48" s="3">
+        <v>0.34417727260539488</v>
+      </c>
+    </row>
+    <row r="49" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0.89678795556632096</v>
+      </c>
+      <c r="F49" s="3">
+        <v>0.29174972745231442</v>
+      </c>
+      <c r="J49" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="K49" s="3">
+        <v>0.90681820918125555</v>
+      </c>
+      <c r="L49" s="3">
+        <v>0.30829801070136592</v>
+      </c>
+    </row>
+    <row r="50" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.89960884324946866</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.25334832780984762</v>
+      </c>
+      <c r="J50" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="K50" s="3">
+        <v>0.90396337711884267</v>
+      </c>
+      <c r="L50" s="3">
+        <v>0.32269804555968251</v>
+      </c>
+    </row>
+    <row r="51" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0.89752875623585315</v>
+      </c>
+      <c r="F51" s="3">
+        <v>0.2936027574149862</v>
+      </c>
+      <c r="J51" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="K51" s="3">
+        <v>0.90693023941997919</v>
+      </c>
+      <c r="L51" s="3">
+        <v>0.33961824834053139</v>
+      </c>
+    </row>
+    <row r="52" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.89871889367819091</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.24065257239927429</v>
+      </c>
+      <c r="J52" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="K52" s="3">
+        <v>0.90674446886971027</v>
+      </c>
+      <c r="L52" s="3">
+        <v>0.35862164817227471</v>
+      </c>
+    </row>
+    <row r="53" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0.89953641535628537</v>
+      </c>
+      <c r="F53" s="3">
+        <v>0.2492218319333441</v>
+      </c>
+      <c r="J53" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="K53" s="3">
+        <v>0.90503412311777087</v>
+      </c>
+      <c r="L53" s="3">
+        <v>0.36070908551586822</v>
+      </c>
+    </row>
+    <row r="54" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="E54" s="3">
+        <v>0.89810189952562303</v>
+      </c>
+      <c r="F54" s="3">
+        <v>0.28298325700822508</v>
+      </c>
+      <c r="J54" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="K54" s="3">
+        <v>0.9062280592663311</v>
+      </c>
+      <c r="L54" s="3">
+        <v>0.35826711604088057</v>
+      </c>
+    </row>
+    <row r="55" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D55" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0.89890230050206288</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0.26993216906255901</v>
+      </c>
+      <c r="J55" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="K55" s="3">
+        <v>0.904524870314658</v>
+      </c>
+      <c r="L55" s="3">
+        <v>0.32981012043012192</v>
+      </c>
+    </row>
+    <row r="57" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="3">
+        <f>AVERAGE(E6:E55)</f>
+        <v>0.89778033710939609</v>
+      </c>
+      <c r="F57" s="3">
+        <f>AVERAGE(F6:F55)</f>
+        <v>0.27573117297695088</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K57" s="3">
+        <f>AVERAGE(K6:K55)</f>
+        <v>0.90602557041699849</v>
+      </c>
+      <c r="L57" s="3">
+        <f>AVERAGE(L6:L55)</f>
+        <v>0.32503056967694349</v>
+      </c>
+    </row>
+    <row r="58" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="3">
+        <f>_xlfn.STDEV.S(E6:E55)</f>
+        <v>1.2790642900937243E-3</v>
+      </c>
+      <c r="F58" s="3">
+        <f>_xlfn.STDEV.S(F6:F55)</f>
+        <v>2.1958553241676768E-2</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K58" s="3">
+        <f>_xlfn.STDEV.S(K6:K55)</f>
+        <v>1.379915286741316E-3</v>
+      </c>
+      <c r="L58" s="3">
+        <f>_xlfn.STDEV.S(L6:L55)</f>
+        <v>2.2127364474893569E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:P32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2767,9 +4118,10 @@
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2779,8 +4131,20 @@
       <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
@@ -2790,8 +4154,20 @@
       <c r="D5" s="3">
         <v>3.5839162327457257E-2</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="3">
+        <v>5.9488779016518112E-2</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="3">
+        <v>2.9884759031708862E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2801,8 +4177,20 @@
       <c r="D6" s="3">
         <v>4.6028263868876838E-2</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="3">
+        <v>5.5610458398160881E-2</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="P6" s="3">
+        <v>2.3824907865479202E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
@@ -2812,8 +4200,20 @@
       <c r="D7" s="3">
         <v>5.648927896701416E-2</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="3">
+        <v>6.0403418239606731E-2</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="P7" s="3">
+        <v>2.5124802420021169E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
@@ -2823,8 +4223,20 @@
       <c r="D8" s="3">
         <v>0.14226226591072541</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="3">
+        <v>5.6977217942613061E-2</v>
+      </c>
+      <c r="O8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" s="3">
+        <v>3.7911740382224272E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
@@ -2834,8 +4246,20 @@
       <c r="D9" s="3">
         <v>0.1490336878608037</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="3">
+        <v>8.4446572990212146E-2</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" s="3">
+        <v>4.8602959606299692E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
@@ -2845,8 +4269,20 @@
       <c r="D10" s="3">
         <v>3.2349520015093267E-2</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="L10" s="3">
+        <v>5.8505404289282373E-2</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="3">
+        <v>3.0391294166711911E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
@@ -2856,8 +4292,20 @@
       <c r="D11" s="3">
         <v>3.687169044121625E-2</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.14193218019964149</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P11" s="3">
+        <v>7.6725442774408584E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
@@ -2867,8 +4315,20 @@
       <c r="D12" s="3">
         <v>5.4983417701167853E-2</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="3">
+        <v>7.4003184006731851E-2</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="P12" s="3">
+        <v>4.2689366802183007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
@@ -2878,8 +4338,20 @@
       <c r="D13" s="3">
         <v>0.1000667937501426</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="3">
+        <v>8.0522762607605408E-2</v>
+      </c>
+      <c r="O13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="P13" s="3">
+        <v>3.7627777925334213E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
@@ -2889,8 +4361,20 @@
       <c r="D14" s="3">
         <v>6.5429969665446008E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" s="3">
+        <v>6.6036902776701212E-2</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" s="3">
+        <v>3.1719670398973457E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
@@ -2900,8 +4384,20 @@
       <c r="D15" s="3">
         <v>3.822299269172038E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="3">
+        <v>5.8791167678081721E-2</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="P15" s="3">
+        <v>3.552658184529725E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
@@ -2911,8 +4407,20 @@
       <c r="D16" s="3">
         <v>4.1288856968829481E-2</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="3">
+        <v>9.0149449777747734E-2</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P16" s="3">
+        <v>9.7923259736975521E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2922,8 +4430,20 @@
       <c r="D17" s="3">
         <v>0.1120867822496293</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" s="3">
+        <v>5.4494961146640888E-2</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="P17" s="3">
+        <v>2.9238202951780569E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>21</v>
       </c>
@@ -2933,8 +4453,20 @@
       <c r="D18" s="3">
         <v>4.0743905516229313E-2</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="K18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" s="3">
+        <v>5.8637540930456387E-2</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="P18" s="3">
+        <v>2.375557566817026E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
@@ -2944,11 +4476,120 @@
       <c r="D19" s="3">
         <v>4.8303412065648192E-2</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="O19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="P19" s="3">
+        <v>2.8114733218078121E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D20" s="6"/>
+      <c r="O20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P20" s="3">
+        <v>3.2802825469900987E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O21" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="P21" s="3">
+        <v>3.5332766189128867E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="P22" s="3">
+        <v>3.2769620441415959E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P23" s="3">
+        <v>4.1648676160846762E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O24" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="P24" s="3">
+        <v>3.4158862614362233E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O25" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P25" s="3">
+        <v>3.249785324545075E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P26" s="3">
+        <v>3.4122402443515901E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O27" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="P27" s="3">
+        <v>3.233685814745544E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O28" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="P28" s="3">
+        <v>2.9273473008173921E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O29" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="P29" s="3">
+        <v>2.2377191968737369E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O30" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P30" s="3">
+        <v>2.4356895550089741E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O31" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="P31" s="3">
+        <v>2.4808400569703098E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="P32" s="3">
+        <v>2.445309939757288E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
xgboost and rf (mse)
</commit_message>
<xml_diff>
--- a/migforecasting/social conflicts/test for paper.xlsx
+++ b/migforecasting/social conflicts/test for paper.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="80">
   <si>
     <t>train (R2)</t>
   </si>
@@ -253,6 +253,15 @@
   </si>
   <si>
     <t>XGBoost</t>
+  </si>
+  <si>
+    <t>NN (128*4-&gt;1, e=100, b=10, relu, mse)</t>
+  </si>
+  <si>
+    <t>train (MSE)</t>
+  </si>
+  <si>
+    <t>test (MSE)</t>
   </si>
 </sst>
 </file>
@@ -2623,10 +2632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:AG57"/>
+  <dimension ref="C1:AT57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2635,9 +2644,10 @@
     <col min="16" max="16" width="11.28515625" customWidth="1"/>
     <col min="20" max="20" width="11.28515625" customWidth="1"/>
     <col min="21" max="21" width="12.28515625" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2647,17 +2657,26 @@
       <c r="M1" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="U1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AR1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2670,20 +2689,32 @@
         <v>5</v>
       </c>
       <c r="O2" s="1"/>
+      <c r="Q2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="1"/>
       <c r="U2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="W2" s="1"/>
-      <c r="Z2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="1"/>
-      <c r="AE2" s="1" t="s">
+      <c r="AA2" s="1"/>
+      <c r="AH2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AG2" s="1"/>
-    </row>
-    <row r="3" spans="3:33" x14ac:dyDescent="0.25">
+      <c r="AJ2" s="1"/>
+      <c r="AM2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO2" s="1"/>
+      <c r="AR2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT2" s="1"/>
+    </row>
+    <row r="3" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
@@ -2693,17 +2724,26 @@
       <c r="M3" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="Q3" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="U3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AH3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AM3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AR3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -2725,29 +2765,50 @@
       <c r="O4" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="U4" s="2"/>
       <c r="V4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="2" t="s">
+      <c r="AJ4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2" t="s">
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB4" s="2" t="s">
+      <c r="AO4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2" t="s">
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AG4" s="2" t="s">
+      <c r="AT4" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -2770,40 +2831,67 @@
         <v>1</v>
       </c>
       <c r="N5" s="3">
-        <v>0.5729003942191212</v>
+        <v>0.96376463714200022</v>
       </c>
       <c r="O5" s="3">
-        <v>0.43373143217207027</v>
+        <v>0.62359503562562546</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0.93059818350705847</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0.58051363350021623</v>
       </c>
       <c r="U5" s="2">
         <v>1</v>
       </c>
       <c r="V5" s="3">
+        <v>1.5034625322084961E-2</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0.10253386685648069</v>
+      </c>
+      <c r="Y5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>9.7254411034077507E-3</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0.11570172630398649</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="3">
         <v>0.9483826461959044</v>
       </c>
-      <c r="W5" s="3">
+      <c r="AJ5" s="3">
         <v>0.62424276749922858</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AM5" s="2">
         <v>1</v>
       </c>
-      <c r="AA5" s="3">
+      <c r="AN5" s="3">
         <v>0.11629864236609461</v>
       </c>
-      <c r="AB5" s="3">
+      <c r="AO5" s="3">
         <v>0.31224638203978711</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="AR5" s="2">
         <v>1</v>
       </c>
-      <c r="AF5" s="3">
+      <c r="AS5" s="3">
         <v>8.1769613043519596E-2</v>
       </c>
-      <c r="AG5" s="3">
+      <c r="AT5" s="3">
         <v>0.2185752247090387</v>
       </c>
     </row>
-    <row r="6" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -2829,43 +2917,73 @@
         <v>2</v>
       </c>
       <c r="N6" s="3">
-        <v>0.57014393347583381</v>
+        <v>0.96804475655403921</v>
       </c>
       <c r="O6" s="3">
-        <v>0.43618552280823431</v>
+        <v>0.66502481796723922</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>Q5+1</f>
+        <v>2</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0.93456370580028147</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0.64161757131163344</v>
       </c>
       <c r="U6" s="2">
         <f>U5+1</f>
         <v>2</v>
       </c>
       <c r="V6" s="3">
+        <v>1.4764452034542481E-2</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0.10843676886549219</v>
+      </c>
+      <c r="Y6" s="2">
+        <f>Y5+1</f>
+        <v>2</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>1.0216734570977571E-2</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0.1110102435603075</v>
+      </c>
+      <c r="AH6" s="2">
+        <f>AH5+1</f>
+        <v>2</v>
+      </c>
+      <c r="AI6" s="3">
         <v>0.95014181806151399</v>
       </c>
-      <c r="W6" s="3">
+      <c r="AJ6" s="3">
         <v>0.65165738632552261</v>
       </c>
-      <c r="Z6" s="2">
-        <f>Z5+1</f>
+      <c r="AM6" s="2">
+        <f>AM5+1</f>
         <v>2</v>
       </c>
-      <c r="AA6" s="3">
+      <c r="AN6" s="3">
         <v>0.1168169117142514</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AO6" s="3">
         <v>0.31273421380824667</v>
       </c>
-      <c r="AE6" s="2">
-        <f>AE5+1</f>
+      <c r="AR6" s="2">
+        <f>AR5+1</f>
         <v>2</v>
       </c>
-      <c r="AF6" s="3">
+      <c r="AS6" s="3">
         <v>8.2015583435031403E-2</v>
       </c>
-      <c r="AG6" s="3">
+      <c r="AT6" s="3">
         <v>0.228059986916406</v>
       </c>
     </row>
-    <row r="7" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -2891,43 +3009,73 @@
         <v>3</v>
       </c>
       <c r="N7" s="3">
-        <v>0.56924440784655839</v>
+        <v>0.96645022569360428</v>
       </c>
       <c r="O7" s="3">
-        <v>0.44454614706989459</v>
+        <v>0.63576930319603719</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" ref="Q7:Q24" si="3">Q6+1</f>
+        <v>3</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0.92751102854144163</v>
+      </c>
+      <c r="S7" s="3">
+        <v>0.67724501933630687</v>
       </c>
       <c r="U7" s="2">
-        <f t="shared" ref="U7:U54" si="3">U6+1</f>
+        <f t="shared" ref="U7:U24" si="4">U6+1</f>
         <v>3</v>
       </c>
       <c r="V7" s="3">
+        <v>1.524398996920061E-2</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0.1018896244447343</v>
+      </c>
+      <c r="Y7" s="2">
+        <f t="shared" ref="Y7:Y24" si="5">Y6+1</f>
+        <v>3</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>1.028121426492695E-2</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>0.1160347139259587</v>
+      </c>
+      <c r="AH7" s="2">
+        <f t="shared" ref="AH7:AH54" si="6">AH6+1</f>
+        <v>3</v>
+      </c>
+      <c r="AI7" s="3">
         <v>0.94851326772255407</v>
       </c>
-      <c r="W7" s="3">
+      <c r="AJ7" s="3">
         <v>0.6671959229934028</v>
       </c>
-      <c r="Z7" s="2">
-        <f t="shared" ref="Z7:Z54" si="4">Z6+1</f>
+      <c r="AM7" s="2">
+        <f t="shared" ref="AM7:AM54" si="7">AM6+1</f>
         <v>3</v>
       </c>
-      <c r="AA7" s="3">
+      <c r="AN7" s="3">
         <v>0.1179096055996649</v>
       </c>
-      <c r="AB7" s="3">
+      <c r="AO7" s="3">
         <v>0.29563574077515559</v>
       </c>
-      <c r="AE7" s="2">
-        <f t="shared" ref="AE7:AE54" si="5">AE6+1</f>
+      <c r="AR7" s="2">
+        <f t="shared" ref="AR7:AR54" si="8">AR6+1</f>
         <v>3</v>
       </c>
-      <c r="AF7" s="3">
+      <c r="AS7" s="3">
         <v>8.2242710734438632E-2</v>
       </c>
-      <c r="AG7" s="3">
+      <c r="AT7" s="3">
         <v>0.2149826377335019</v>
       </c>
     </row>
-    <row r="8" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2953,43 +3101,73 @@
         <v>4</v>
       </c>
       <c r="N8" s="3">
-        <v>0.54245416236916832</v>
+        <v>0.96658039969724063</v>
       </c>
       <c r="O8" s="3">
-        <v>0.48360989825138317</v>
-      </c>
-      <c r="U8" s="2">
+        <v>0.67227564588948074</v>
+      </c>
+      <c r="Q8" s="2">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="V8" s="3">
-        <v>0.94974359082717996</v>
-      </c>
-      <c r="W8" s="3">
-        <v>0.62610975868051677</v>
-      </c>
-      <c r="Z8" s="2">
+      <c r="R8" s="3">
+        <v>0.90509582258875232</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0.66056614603622676</v>
+      </c>
+      <c r="U8" s="2">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="AA8" s="3">
-        <v>0.1172464566941234</v>
-      </c>
-      <c r="AB8" s="3">
-        <v>0.30646210688982789</v>
-      </c>
-      <c r="AE8" s="2">
+      <c r="V8" s="3">
+        <v>1.530080098197413E-2</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0.1021724876171361</v>
+      </c>
+      <c r="Y8" s="2">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AF8" s="3">
+      <c r="Z8" s="3">
+        <v>1.163661095152236E-2</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0.1048205338783237</v>
+      </c>
+      <c r="AH8" s="2">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AI8" s="3">
+        <v>0.94974359082717996</v>
+      </c>
+      <c r="AJ8" s="3">
+        <v>0.62610975868051677</v>
+      </c>
+      <c r="AM8" s="2">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="AN8" s="3">
+        <v>0.1172464566941234</v>
+      </c>
+      <c r="AO8" s="3">
+        <v>0.30646210688982789</v>
+      </c>
+      <c r="AR8" s="2">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AS8" s="3">
         <v>8.1549176794793454E-2</v>
       </c>
-      <c r="AG8" s="3">
+      <c r="AT8" s="3">
         <v>0.22654039805285689</v>
       </c>
     </row>
-    <row r="9" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3015,43 +3193,73 @@
         <v>5</v>
       </c>
       <c r="N9" s="3">
-        <v>0.5647076339167596</v>
+        <v>0.96495952318547551</v>
       </c>
       <c r="O9" s="3">
-        <v>0.43857857430598168</v>
-      </c>
-      <c r="U9" s="2">
+        <v>0.67137239596803533</v>
+      </c>
+      <c r="Q9" s="2">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="V9" s="3">
-        <v>0.95025250774461234</v>
-      </c>
-      <c r="W9" s="3">
-        <v>0.62707359060358336</v>
-      </c>
-      <c r="Z9" s="2">
+      <c r="R9" s="3">
+        <v>0.91760974646496485</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0.67547158883915204</v>
+      </c>
+      <c r="U9" s="2">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="AA9" s="3">
-        <v>0.11815620674558699</v>
-      </c>
-      <c r="AB9" s="3">
-        <v>0.30697978105111479</v>
-      </c>
-      <c r="AE9" s="2">
+      <c r="V9" s="3">
+        <v>1.489262305778513E-2</v>
+      </c>
+      <c r="W9" s="3">
+        <v>9.8546136415411351E-2</v>
+      </c>
+      <c r="Y9" s="2">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="AF9" s="3">
+      <c r="Z9" s="3">
+        <v>9.5377722088051623E-3</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0.1052218865180526</v>
+      </c>
+      <c r="AH9" s="2">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="AI9" s="3">
+        <v>0.95025250774461234</v>
+      </c>
+      <c r="AJ9" s="3">
+        <v>0.62707359060358336</v>
+      </c>
+      <c r="AM9" s="2">
+        <f t="shared" si="7"/>
+        <v>5</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>0.11815620674558699</v>
+      </c>
+      <c r="AO9" s="3">
+        <v>0.30697978105111479</v>
+      </c>
+      <c r="AR9" s="2">
+        <f t="shared" si="8"/>
+        <v>5</v>
+      </c>
+      <c r="AS9" s="3">
         <v>8.1536264136596287E-2</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AT9" s="3">
         <v>0.22159406681404359</v>
       </c>
     </row>
-    <row r="10" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3077,43 +3285,73 @@
         <v>6</v>
       </c>
       <c r="N10" s="3">
-        <v>0.56519497361366344</v>
+        <v>0.96554140647002118</v>
       </c>
       <c r="O10" s="3">
-        <v>0.49003408102072449</v>
-      </c>
-      <c r="U10" s="2">
+        <v>0.6474584870092972</v>
+      </c>
+      <c r="Q10" s="2">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="V10" s="3">
-        <v>0.94796415952673541</v>
-      </c>
-      <c r="W10" s="3">
-        <v>0.67429355017169756</v>
-      </c>
-      <c r="Z10" s="2">
+      <c r="R10" s="3">
+        <v>0.91006532245050487</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0.67981396316488496</v>
+      </c>
+      <c r="U10" s="2">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="AA10" s="3">
-        <v>0.1169240315092835</v>
-      </c>
-      <c r="AB10" s="3">
-        <v>0.30980523001355198</v>
-      </c>
-      <c r="AE10" s="2">
+      <c r="V10" s="3">
+        <v>1.476850552290742E-2</v>
+      </c>
+      <c r="W10" s="3">
+        <v>0.1075442703430376</v>
+      </c>
+      <c r="Y10" s="2">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="AF10" s="3">
+      <c r="Z10" s="3">
+        <v>1.0286084904980919E-2</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>0.12026798540613259</v>
+      </c>
+      <c r="AH10" s="2">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="AI10" s="3">
+        <v>0.94796415952673541</v>
+      </c>
+      <c r="AJ10" s="3">
+        <v>0.67429355017169756</v>
+      </c>
+      <c r="AM10" s="2">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="AN10" s="3">
+        <v>0.1169240315092835</v>
+      </c>
+      <c r="AO10" s="3">
+        <v>0.30980523001355198</v>
+      </c>
+      <c r="AR10" s="2">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="AS10" s="3">
         <v>8.1823070141145773E-2</v>
       </c>
-      <c r="AG10" s="3">
+      <c r="AT10" s="3">
         <v>0.22855806711828469</v>
       </c>
     </row>
-    <row r="11" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3139,43 +3377,73 @@
         <v>7</v>
       </c>
       <c r="N11" s="3">
-        <v>0.57312800073621273</v>
+        <v>0.96745516133544252</v>
       </c>
       <c r="O11" s="3">
-        <v>0.46137825217904482</v>
-      </c>
-      <c r="U11" s="2">
+        <v>0.63782181397582938</v>
+      </c>
+      <c r="Q11" s="2">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="V11" s="3">
-        <v>0.94938913654931145</v>
-      </c>
-      <c r="W11" s="3">
-        <v>0.64531580148263057</v>
-      </c>
-      <c r="Z11" s="2">
+      <c r="R11" s="3">
+        <v>0.90903325184805839</v>
+      </c>
+      <c r="S11" s="3">
+        <v>0.65572288566889669</v>
+      </c>
+      <c r="U11" s="2">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="AA11" s="3">
-        <v>0.1162986700492049</v>
-      </c>
-      <c r="AB11" s="3">
-        <v>0.32155039855673279</v>
-      </c>
-      <c r="AE11" s="2">
+      <c r="V11" s="3">
+        <v>1.4712986857944071E-2</v>
+      </c>
+      <c r="W11" s="3">
+        <v>0.1076780221436838</v>
+      </c>
+      <c r="Y11" s="2">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="AF11" s="3">
+      <c r="Z11" s="3">
+        <v>9.7967090279293435E-3</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>0.1044312865263093</v>
+      </c>
+      <c r="AH11" s="2">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="AI11" s="3">
+        <v>0.94938913654931145</v>
+      </c>
+      <c r="AJ11" s="3">
+        <v>0.64531580148263057</v>
+      </c>
+      <c r="AM11" s="2">
+        <f t="shared" si="7"/>
+        <v>7</v>
+      </c>
+      <c r="AN11" s="3">
+        <v>0.1162986700492049</v>
+      </c>
+      <c r="AO11" s="3">
+        <v>0.32155039855673279</v>
+      </c>
+      <c r="AR11" s="2">
+        <f t="shared" si="8"/>
+        <v>7</v>
+      </c>
+      <c r="AS11" s="3">
         <v>8.1705863850174379E-2</v>
       </c>
-      <c r="AG11" s="3">
+      <c r="AT11" s="3">
         <v>0.21721269051565181</v>
       </c>
     </row>
-    <row r="12" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3201,43 +3469,73 @@
         <v>8</v>
       </c>
       <c r="N12" s="3">
-        <v>0.56548886907172435</v>
+        <v>0.96867666625655269</v>
       </c>
       <c r="O12" s="3">
-        <v>0.46364370417685119</v>
-      </c>
-      <c r="U12" s="2">
+        <v>0.65038652061124136</v>
+      </c>
+      <c r="Q12" s="2">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="V12" s="3">
-        <v>0.94858419153504725</v>
-      </c>
-      <c r="W12" s="3">
-        <v>0.62639699780051294</v>
-      </c>
-      <c r="Z12" s="2">
+      <c r="R12" s="3">
+        <v>0.93874239846378771</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0.67022182967905586</v>
+      </c>
+      <c r="U12" s="2">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="AA12" s="3">
-        <v>0.11776354951009541</v>
-      </c>
-      <c r="AB12" s="3">
-        <v>0.31911434022278012</v>
-      </c>
-      <c r="AE12" s="2">
+      <c r="V12" s="3">
+        <v>1.5026179545689621E-2</v>
+      </c>
+      <c r="W12" s="3">
+        <v>0.10030747828149369</v>
+      </c>
+      <c r="Y12" s="2">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="AF12" s="3">
+      <c r="Z12" s="3">
+        <v>1.0141614466680261E-2</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>9.4813154183915338E-2</v>
+      </c>
+      <c r="AH12" s="2">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>0.94858419153504725</v>
+      </c>
+      <c r="AJ12" s="3">
+        <v>0.62639699780051294</v>
+      </c>
+      <c r="AM12" s="2">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="AN12" s="3">
+        <v>0.11776354951009541</v>
+      </c>
+      <c r="AO12" s="3">
+        <v>0.31911434022278012</v>
+      </c>
+      <c r="AR12" s="2">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="AS12" s="3">
         <v>8.2664068657790857E-2</v>
       </c>
-      <c r="AG12" s="3">
+      <c r="AT12" s="3">
         <v>0.21594411354817489</v>
       </c>
     </row>
-    <row r="13" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3263,43 +3561,73 @@
         <v>9</v>
       </c>
       <c r="N13" s="3">
-        <v>0.56569296433728455</v>
+        <v>0.96774542035502986</v>
       </c>
       <c r="O13" s="3">
-        <v>0.471774283102813</v>
-      </c>
-      <c r="U13" s="2">
+        <v>0.65614073554898811</v>
+      </c>
+      <c r="Q13" s="2">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="V13" s="3">
-        <v>0.94893636270296566</v>
-      </c>
-      <c r="W13" s="3">
-        <v>0.66640684057230692</v>
-      </c>
-      <c r="Z13" s="2">
+      <c r="R13" s="3">
+        <v>0.90286621421309232</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0.64378713132094623</v>
+      </c>
+      <c r="U13" s="2">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="AA13" s="3">
-        <v>0.1156787760033966</v>
-      </c>
-      <c r="AB13" s="3">
-        <v>0.31468487648743998</v>
-      </c>
-      <c r="AE13" s="2">
+      <c r="V13" s="3">
+        <v>1.485988747458407E-2</v>
+      </c>
+      <c r="W13" s="3">
+        <v>0.1138696459166669</v>
+      </c>
+      <c r="Y13" s="2">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="AF13" s="3">
+      <c r="Z13" s="3">
+        <v>1.020521913866438E-2</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>0.106946473612236</v>
+      </c>
+      <c r="AH13" s="2">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>0.94893636270296566</v>
+      </c>
+      <c r="AJ13" s="3">
+        <v>0.66640684057230692</v>
+      </c>
+      <c r="AM13" s="2">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="AN13" s="3">
+        <v>0.1156787760033966</v>
+      </c>
+      <c r="AO13" s="3">
+        <v>0.31468487648743998</v>
+      </c>
+      <c r="AR13" s="2">
+        <f t="shared" si="8"/>
+        <v>9</v>
+      </c>
+      <c r="AS13" s="3">
         <v>8.2246020605867914E-2</v>
       </c>
-      <c r="AG13" s="3">
+      <c r="AT13" s="3">
         <v>0.22114865492312391</v>
       </c>
     </row>
-    <row r="14" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3325,43 +3653,73 @@
         <v>10</v>
       </c>
       <c r="N14" s="3">
-        <v>0.56131778126338294</v>
+        <v>0.96695142665664691</v>
       </c>
       <c r="O14" s="3">
-        <v>0.49331047699419939</v>
-      </c>
-      <c r="U14" s="2">
+        <v>0.58497164771542542</v>
+      </c>
+      <c r="Q14" s="2">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="V14" s="3">
-        <v>0.95029434903033028</v>
-      </c>
-      <c r="W14" s="3">
-        <v>0.63156679502402269</v>
-      </c>
-      <c r="Z14" s="2">
+      <c r="R14" s="3">
+        <v>0.93063588370645434</v>
+      </c>
+      <c r="S14" s="3">
+        <v>0.66387289968503982</v>
+      </c>
+      <c r="U14" s="2">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="AA14" s="3">
-        <v>0.1178000635324878</v>
-      </c>
-      <c r="AB14" s="3">
-        <v>0.30004516193868969</v>
-      </c>
-      <c r="AE14" s="2">
+      <c r="V14" s="3">
+        <v>1.487784831102958E-2</v>
+      </c>
+      <c r="W14" s="3">
+        <v>0.1031935406231308</v>
+      </c>
+      <c r="Y14" s="2">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="AF14" s="3">
+      <c r="Z14" s="3">
+        <v>9.6083974809740222E-3</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>0.1113686452837185</v>
+      </c>
+      <c r="AH14" s="2">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="AI14" s="3">
+        <v>0.95029434903033028</v>
+      </c>
+      <c r="AJ14" s="3">
+        <v>0.63156679502402269</v>
+      </c>
+      <c r="AM14" s="2">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="AN14" s="3">
+        <v>0.1178000635324878</v>
+      </c>
+      <c r="AO14" s="3">
+        <v>0.30004516193868969</v>
+      </c>
+      <c r="AR14" s="2">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="AS14" s="3">
         <v>8.2762723030266369E-2</v>
       </c>
-      <c r="AG14" s="3">
+      <c r="AT14" s="3">
         <v>0.22181721225600909</v>
       </c>
     </row>
-    <row r="15" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3387,43 +3745,73 @@
         <v>11</v>
       </c>
       <c r="N15" s="3">
-        <v>0.5599312129266768</v>
+        <v>0.96817186145221468</v>
       </c>
       <c r="O15" s="3">
-        <v>0.47549414611864671</v>
-      </c>
-      <c r="U15" s="2">
+        <v>0.6632362359115116</v>
+      </c>
+      <c r="Q15" s="2">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="V15" s="3">
-        <v>0.9484002184287218</v>
-      </c>
-      <c r="W15" s="3">
-        <v>0.64802503096297781</v>
-      </c>
-      <c r="Z15" s="2">
+      <c r="R15" s="3">
+        <v>0.92299317362426891</v>
+      </c>
+      <c r="S15" s="3">
+        <v>0.68000886033185592</v>
+      </c>
+      <c r="U15" s="2">
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="AA15" s="3">
-        <v>0.1171383818317885</v>
-      </c>
-      <c r="AB15" s="3">
-        <v>0.30811545296515908</v>
-      </c>
-      <c r="AE15" s="2">
+      <c r="V15" s="3">
+        <v>1.455115476928368E-2</v>
+      </c>
+      <c r="W15" s="3">
+        <v>0.1139143759740549</v>
+      </c>
+      <c r="Y15" s="2">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="AF15" s="3">
+      <c r="Z15" s="3">
+        <v>1.060237720085286E-2</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>9.8518028121507784E-2</v>
+      </c>
+      <c r="AH15" s="2">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
+      <c r="AI15" s="3">
+        <v>0.9484002184287218</v>
+      </c>
+      <c r="AJ15" s="3">
+        <v>0.64802503096297781</v>
+      </c>
+      <c r="AM15" s="2">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+      <c r="AN15" s="3">
+        <v>0.1171383818317885</v>
+      </c>
+      <c r="AO15" s="3">
+        <v>0.30811545296515908</v>
+      </c>
+      <c r="AR15" s="2">
+        <f t="shared" si="8"/>
+        <v>11</v>
+      </c>
+      <c r="AS15" s="3">
         <v>8.3102819747522774E-2</v>
       </c>
-      <c r="AG15" s="3">
+      <c r="AT15" s="3">
         <v>0.2112029915425882</v>
       </c>
     </row>
-    <row r="16" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3449,43 +3837,73 @@
         <v>12</v>
       </c>
       <c r="N16" s="3">
-        <v>0.56888447789891305</v>
+        <v>0.96595701096541908</v>
       </c>
       <c r="O16" s="3">
-        <v>0.46157035683934428</v>
-      </c>
-      <c r="U16" s="2">
+        <v>0.66700725715383224</v>
+      </c>
+      <c r="Q16" s="2">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="V16" s="3">
-        <v>0.94989129262824368</v>
-      </c>
-      <c r="W16" s="3">
-        <v>0.63875755894633546</v>
-      </c>
-      <c r="Z16" s="2">
+      <c r="R16" s="3">
+        <v>0.92046359789099963</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0.6521985590802033</v>
+      </c>
+      <c r="U16" s="2">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="AA16" s="3">
-        <v>0.1171186160910848</v>
-      </c>
-      <c r="AB16" s="3">
-        <v>0.31103563353080099</v>
-      </c>
-      <c r="AE16" s="2">
+      <c r="V16" s="3">
+        <v>1.539029131656122E-2</v>
+      </c>
+      <c r="W16" s="3">
+        <v>9.5257247816083399E-2</v>
+      </c>
+      <c r="Y16" s="2">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="AF16" s="3">
+      <c r="Z16" s="3">
+        <v>9.439217120172861E-3</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>0.11145067949458611</v>
+      </c>
+      <c r="AH16" s="2">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>0.94989129262824368</v>
+      </c>
+      <c r="AJ16" s="3">
+        <v>0.63875755894633546</v>
+      </c>
+      <c r="AM16" s="2">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="AN16" s="3">
+        <v>0.1171186160910848</v>
+      </c>
+      <c r="AO16" s="3">
+        <v>0.31103563353080099</v>
+      </c>
+      <c r="AR16" s="2">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="AS16" s="3">
         <v>8.2339487334254086E-2</v>
       </c>
-      <c r="AG16" s="3">
+      <c r="AT16" s="3">
         <v>0.2260417239367816</v>
       </c>
     </row>
-    <row r="17" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3511,43 +3929,73 @@
         <v>13</v>
       </c>
       <c r="N17" s="3">
-        <v>0.55481490217184271</v>
+        <v>0.968334991632671</v>
       </c>
       <c r="O17" s="3">
-        <v>0.43935771227128562</v>
-      </c>
-      <c r="U17" s="2">
+        <v>0.64718254910704776</v>
+      </c>
+      <c r="Q17" s="2">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="V17" s="3">
-        <v>0.9492074765160603</v>
-      </c>
-      <c r="W17" s="3">
-        <v>0.64812073080130728</v>
-      </c>
-      <c r="Z17" s="2">
+      <c r="R17" s="3">
+        <v>0.92741306163233084</v>
+      </c>
+      <c r="S17" s="3">
+        <v>0.69105130796107628</v>
+      </c>
+      <c r="U17" s="2">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="AA17" s="3">
-        <v>0.1171742453010904</v>
-      </c>
-      <c r="AB17" s="3">
-        <v>0.31140957698377753</v>
-      </c>
-      <c r="AE17" s="2">
+      <c r="V17" s="3">
+        <v>1.509463261395547E-2</v>
+      </c>
+      <c r="W17" s="3">
+        <v>9.6457785484444419E-2</v>
+      </c>
+      <c r="Y17" s="2">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="AF17" s="3">
+      <c r="Z17" s="3">
+        <v>1.0197519243926549E-2</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>0.11246199433009429</v>
+      </c>
+      <c r="AH17" s="2">
+        <f t="shared" si="6"/>
+        <v>13</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>0.9492074765160603</v>
+      </c>
+      <c r="AJ17" s="3">
+        <v>0.64812073080130728</v>
+      </c>
+      <c r="AM17" s="2">
+        <f t="shared" si="7"/>
+        <v>13</v>
+      </c>
+      <c r="AN17" s="3">
+        <v>0.1171742453010904</v>
+      </c>
+      <c r="AO17" s="3">
+        <v>0.31140957698377753</v>
+      </c>
+      <c r="AR17" s="2">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="AS17" s="3">
         <v>8.1596317207806829E-2</v>
       </c>
-      <c r="AG17" s="3">
+      <c r="AT17" s="3">
         <v>0.23112952553723701</v>
       </c>
     </row>
-    <row r="18" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3573,43 +4021,73 @@
         <v>14</v>
       </c>
       <c r="N18" s="3">
-        <v>0.56113394375674164</v>
+        <v>0.96686305288697583</v>
       </c>
       <c r="O18" s="3">
-        <v>0.51816536686718728</v>
-      </c>
-      <c r="U18" s="2">
+        <v>0.63392098300799749</v>
+      </c>
+      <c r="Q18" s="2">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="V18" s="3">
-        <v>0.94938848879038751</v>
-      </c>
-      <c r="W18" s="3">
-        <v>0.66775707346954982</v>
-      </c>
-      <c r="Z18" s="2">
+      <c r="R18" s="3">
+        <v>0.91881001221897252</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0.61515329388807605</v>
+      </c>
+      <c r="U18" s="2">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="AA18" s="3">
-        <v>0.1164586784263299</v>
-      </c>
-      <c r="AB18" s="3">
-        <v>0.30973552394199477</v>
-      </c>
-      <c r="AE18" s="2">
+      <c r="V18" s="3">
+        <v>1.501486089602681E-2</v>
+      </c>
+      <c r="W18" s="3">
+        <v>0.1017507957212412</v>
+      </c>
+      <c r="Y18" s="2">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="AF18" s="3">
+      <c r="Z18" s="3">
+        <v>9.9459032013071696E-3</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>0.1187995999173132</v>
+      </c>
+      <c r="AH18" s="2">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="AI18" s="3">
+        <v>0.94938848879038751</v>
+      </c>
+      <c r="AJ18" s="3">
+        <v>0.66775707346954982</v>
+      </c>
+      <c r="AM18" s="2">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="AN18" s="3">
+        <v>0.1164586784263299</v>
+      </c>
+      <c r="AO18" s="3">
+        <v>0.30973552394199477</v>
+      </c>
+      <c r="AR18" s="2">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="AS18" s="3">
         <v>8.2632752639061433E-2</v>
       </c>
-      <c r="AG18" s="3">
+      <c r="AT18" s="3">
         <v>0.21940649077523819</v>
       </c>
     </row>
-    <row r="19" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3635,43 +4113,73 @@
         <v>15</v>
       </c>
       <c r="N19" s="3">
-        <v>0.55820316769467215</v>
+        <v>0.96725845511840991</v>
       </c>
       <c r="O19" s="3">
-        <v>0.5041717052889565</v>
-      </c>
-      <c r="U19" s="2">
+        <v>0.63237481941050588</v>
+      </c>
+      <c r="Q19" s="2">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="V19" s="3">
-        <v>0.94881345044029819</v>
-      </c>
-      <c r="W19" s="3">
-        <v>0.61746215094387957</v>
-      </c>
-      <c r="Z19" s="2">
+      <c r="R19" s="3">
+        <v>0.92446872839028571</v>
+      </c>
+      <c r="S19" s="3">
+        <v>0.65414577345870517</v>
+      </c>
+      <c r="U19" s="2">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="AA19" s="3">
-        <v>0.1177906235918996</v>
-      </c>
-      <c r="AB19" s="3">
-        <v>0.30600599996569089</v>
-      </c>
-      <c r="AE19" s="2">
+      <c r="V19" s="3">
+        <v>1.51731811306664E-2</v>
+      </c>
+      <c r="W19" s="3">
+        <v>0.10248288858187091</v>
+      </c>
+      <c r="Y19" s="2">
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="AF19" s="3">
+      <c r="Z19" s="3">
+        <v>1.0488520383780319E-2</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>9.6080827079211756E-2</v>
+      </c>
+      <c r="AH19" s="2">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="AI19" s="3">
+        <v>0.94881345044029819</v>
+      </c>
+      <c r="AJ19" s="3">
+        <v>0.61746215094387957</v>
+      </c>
+      <c r="AM19" s="2">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="AN19" s="3">
+        <v>0.1177906235918996</v>
+      </c>
+      <c r="AO19" s="3">
+        <v>0.30600599996569089</v>
+      </c>
+      <c r="AR19" s="2">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="AS19" s="3">
         <v>8.1650285344827836E-2</v>
       </c>
-      <c r="AG19" s="3">
+      <c r="AT19" s="3">
         <v>0.22222848595890529</v>
       </c>
     </row>
-    <row r="20" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3697,43 +4205,73 @@
         <v>16</v>
       </c>
       <c r="N20" s="3">
-        <v>0.55378810396872091</v>
+        <v>0.97056227637556525</v>
       </c>
       <c r="O20" s="3">
-        <v>0.47859722758407591</v>
-      </c>
-      <c r="U20" s="2">
+        <v>0.61294404459202034</v>
+      </c>
+      <c r="Q20" s="2">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="V20" s="3">
-        <v>0.95006313957131971</v>
-      </c>
-      <c r="W20" s="3">
-        <v>0.61314988818603333</v>
-      </c>
-      <c r="Z20" s="2">
+      <c r="R20" s="3">
+        <v>0.92170689584554721</v>
+      </c>
+      <c r="S20" s="3">
+        <v>0.70560113634140675</v>
+      </c>
+      <c r="U20" s="2">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
-      <c r="AA20" s="3">
-        <v>0.11747927165115141</v>
-      </c>
-      <c r="AB20" s="3">
-        <v>0.31312975008720212</v>
-      </c>
-      <c r="AE20" s="2">
+      <c r="V20" s="3">
+        <v>1.524970865159618E-2</v>
+      </c>
+      <c r="W20" s="3">
+        <v>0.1043101435580429</v>
+      </c>
+      <c r="Y20" s="2">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="AF20" s="3">
+      <c r="Z20" s="3">
+        <v>1.063781859124845E-2</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>9.9892162405763318E-2</v>
+      </c>
+      <c r="AH20" s="2">
+        <f t="shared" si="6"/>
+        <v>16</v>
+      </c>
+      <c r="AI20" s="3">
+        <v>0.95006313957131971</v>
+      </c>
+      <c r="AJ20" s="3">
+        <v>0.61314988818603333</v>
+      </c>
+      <c r="AM20" s="2">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="AN20" s="3">
+        <v>0.11747927165115141</v>
+      </c>
+      <c r="AO20" s="3">
+        <v>0.31312975008720212</v>
+      </c>
+      <c r="AR20" s="2">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="AS20" s="3">
         <v>8.2300244262586322E-2</v>
       </c>
-      <c r="AG20" s="3">
+      <c r="AT20" s="3">
         <v>0.2131942670611168</v>
       </c>
     </row>
-    <row r="21" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3759,43 +4297,73 @@
         <v>17</v>
       </c>
       <c r="N21" s="3">
-        <v>0.55925898134961838</v>
+        <v>0.96852328735592308</v>
       </c>
       <c r="O21" s="3">
-        <v>0.49724186270127962</v>
-      </c>
-      <c r="U21" s="2">
+        <v>0.61174912077165566</v>
+      </c>
+      <c r="Q21" s="2">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="V21" s="3">
-        <v>0.94841670021682811</v>
-      </c>
-      <c r="W21" s="3">
-        <v>0.68723334489831167</v>
-      </c>
-      <c r="Z21" s="2">
+      <c r="R21" s="3">
+        <v>0.92248615253204136</v>
+      </c>
+      <c r="S21" s="3">
+        <v>0.65636503240016197</v>
+      </c>
+      <c r="U21" s="2">
         <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="AA21" s="3">
-        <v>0.1170660597063146</v>
-      </c>
-      <c r="AB21" s="3">
-        <v>0.31892808825715768</v>
-      </c>
-      <c r="AE21" s="2">
+      <c r="V21" s="3">
+        <v>1.4829091549765959E-2</v>
+      </c>
+      <c r="W21" s="3">
+        <v>9.5983189204538827E-2</v>
+      </c>
+      <c r="Y21" s="2">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="AF21" s="3">
+      <c r="Z21" s="3">
+        <v>1.1018297986841249E-2</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>0.1017541605419314</v>
+      </c>
+      <c r="AH21" s="2">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="AI21" s="3">
+        <v>0.94841670021682811</v>
+      </c>
+      <c r="AJ21" s="3">
+        <v>0.68723334489831167</v>
+      </c>
+      <c r="AM21" s="2">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="AN21" s="3">
+        <v>0.1170660597063146</v>
+      </c>
+      <c r="AO21" s="3">
+        <v>0.31892808825715768</v>
+      </c>
+      <c r="AR21" s="2">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="AS21" s="3">
         <v>8.2010057078785031E-2</v>
       </c>
-      <c r="AG21" s="3">
+      <c r="AT21" s="3">
         <v>0.22226383573189001</v>
       </c>
     </row>
-    <row r="22" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3821,43 +4389,73 @@
         <v>18</v>
       </c>
       <c r="N22" s="3">
-        <v>0.5700450489036335</v>
+        <v>0.96705382208082158</v>
       </c>
       <c r="O22" s="3">
-        <v>0.42430837265763438</v>
-      </c>
-      <c r="U22" s="2">
+        <v>0.66057191323634612</v>
+      </c>
+      <c r="Q22" s="2">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="V22" s="3">
-        <v>0.94745703865263975</v>
-      </c>
-      <c r="W22" s="3">
-        <v>0.65213060930063704</v>
-      </c>
-      <c r="Z22" s="2">
+      <c r="R22" s="3">
+        <v>0.90585642879592543</v>
+      </c>
+      <c r="S22" s="3">
+        <v>0.69064017982943171</v>
+      </c>
+      <c r="U22" s="2">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="AA22" s="3">
-        <v>0.1190566414304584</v>
-      </c>
-      <c r="AB22" s="3">
-        <v>0.29201141261772301</v>
-      </c>
-      <c r="AE22" s="2">
+      <c r="V22" s="3">
+        <v>1.5182036031579979E-2</v>
+      </c>
+      <c r="W22" s="3">
+        <v>0.10328630616162759</v>
+      </c>
+      <c r="Y22" s="2">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="AF22" s="3">
+      <c r="Z22" s="3">
+        <v>9.1389457530292161E-3</v>
+      </c>
+      <c r="AA22" s="3">
+        <v>0.117986378761315</v>
+      </c>
+      <c r="AH22" s="2">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="AI22" s="3">
+        <v>0.94745703865263975</v>
+      </c>
+      <c r="AJ22" s="3">
+        <v>0.65213060930063704</v>
+      </c>
+      <c r="AM22" s="2">
+        <f t="shared" si="7"/>
+        <v>18</v>
+      </c>
+      <c r="AN22" s="3">
+        <v>0.1190566414304584</v>
+      </c>
+      <c r="AO22" s="3">
+        <v>0.29201141261772301</v>
+      </c>
+      <c r="AR22" s="2">
+        <f t="shared" si="8"/>
+        <v>18</v>
+      </c>
+      <c r="AS22" s="3">
         <v>8.2465725949413093E-2</v>
       </c>
-      <c r="AG22" s="3">
+      <c r="AT22" s="3">
         <v>0.22775780337315041</v>
       </c>
     </row>
-    <row r="23" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3883,43 +4481,73 @@
         <v>19</v>
       </c>
       <c r="N23" s="3">
-        <v>0.56510457249046109</v>
+        <v>0.96842298205967614</v>
       </c>
       <c r="O23" s="3">
-        <v>0.50059267747274117</v>
-      </c>
-      <c r="U23" s="2">
+        <v>0.65680346391451083</v>
+      </c>
+      <c r="Q23" s="2">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="V23" s="3">
-        <v>0.94775393662384277</v>
-      </c>
-      <c r="W23" s="3">
-        <v>0.63138559963267504</v>
-      </c>
-      <c r="Z23" s="2">
+      <c r="R23" s="3">
+        <v>0.90224972257893765</v>
+      </c>
+      <c r="S23" s="3">
+        <v>0.60318153309996181</v>
+      </c>
+      <c r="U23" s="2">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
-      <c r="AA23" s="3">
-        <v>0.1170426397950606</v>
-      </c>
-      <c r="AB23" s="3">
-        <v>0.31211045796856152</v>
-      </c>
-      <c r="AE23" s="2">
+      <c r="V23" s="3">
+        <v>1.48815956325301E-2</v>
+      </c>
+      <c r="W23" s="3">
+        <v>0.1021515480443403</v>
+      </c>
+      <c r="Y23" s="2">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="AF23" s="3">
+      <c r="Z23" s="3">
+        <v>1.0084064008588359E-2</v>
+      </c>
+      <c r="AA23" s="3">
+        <v>0.1110758473543141</v>
+      </c>
+      <c r="AH23" s="2">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="AI23" s="3">
+        <v>0.94775393662384277</v>
+      </c>
+      <c r="AJ23" s="3">
+        <v>0.63138559963267504</v>
+      </c>
+      <c r="AM23" s="2">
+        <f t="shared" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="AN23" s="3">
+        <v>0.1170426397950606</v>
+      </c>
+      <c r="AO23" s="3">
+        <v>0.31211045796856152</v>
+      </c>
+      <c r="AR23" s="2">
+        <f t="shared" si="8"/>
+        <v>19</v>
+      </c>
+      <c r="AS23" s="3">
         <v>8.1284535638414881E-2</v>
       </c>
-      <c r="AG23" s="3">
+      <c r="AT23" s="3">
         <v>0.2249461185399371</v>
       </c>
     </row>
-    <row r="24" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3945,43 +4573,73 @@
         <v>20</v>
       </c>
       <c r="N24" s="3">
-        <v>0.5605271102695718</v>
+        <v>0.96541496944695859</v>
       </c>
       <c r="O24" s="3">
-        <v>0.48448371170967042</v>
-      </c>
-      <c r="U24" s="2">
+        <v>0.64701515331587733</v>
+      </c>
+      <c r="Q24" s="2">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="V24" s="3">
-        <v>0.94822046642134838</v>
-      </c>
-      <c r="W24" s="3">
-        <v>0.69353925357839019</v>
-      </c>
-      <c r="Z24" s="2">
+      <c r="R24" s="3">
+        <v>0.91726800135491149</v>
+      </c>
+      <c r="S24" s="3">
+        <v>0.61267752326283165</v>
+      </c>
+      <c r="U24" s="2">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="AA24" s="3">
-        <v>0.1170295318423671</v>
-      </c>
-      <c r="AB24" s="3">
-        <v>0.30995721028871059</v>
-      </c>
-      <c r="AE24" s="2">
+      <c r="V24" s="3">
+        <v>1.507075257437346E-2</v>
+      </c>
+      <c r="W24" s="3">
+        <v>0.10130090434442909</v>
+      </c>
+      <c r="Y24" s="2">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="AF24" s="3">
+      <c r="Z24" s="3">
+        <v>9.4343814192197409E-3</v>
+      </c>
+      <c r="AA24" s="3">
+        <v>0.10359555667566971</v>
+      </c>
+      <c r="AH24" s="2">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="AI24" s="3">
+        <v>0.94822046642134838</v>
+      </c>
+      <c r="AJ24" s="3">
+        <v>0.69353925357839019</v>
+      </c>
+      <c r="AM24" s="2">
+        <f t="shared" si="7"/>
+        <v>20</v>
+      </c>
+      <c r="AN24" s="3">
+        <v>0.1170295318423671</v>
+      </c>
+      <c r="AO24" s="3">
+        <v>0.30995721028871059</v>
+      </c>
+      <c r="AR24" s="2">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="AS24" s="3">
         <v>8.2756239960734349E-2</v>
       </c>
-      <c r="AG24" s="3">
+      <c r="AT24" s="3">
         <v>0.2251606878609029</v>
       </c>
     </row>
-    <row r="25" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -4007,43 +4665,46 @@
         <v>21</v>
       </c>
       <c r="N25" s="3">
-        <v>0.56943036020671678</v>
+        <v>0.96706089680873031</v>
       </c>
       <c r="O25" s="3">
-        <v>0.45327508196252347</v>
-      </c>
-      <c r="U25" s="2">
-        <f t="shared" si="3"/>
+        <v>0.63699481735453878</v>
+      </c>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="AH25" s="2">
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="V25" s="3">
+      <c r="AI25" s="3">
         <v>0.94931379914042635</v>
       </c>
-      <c r="W25" s="3">
+      <c r="AJ25" s="3">
         <v>0.62472045871967519</v>
       </c>
-      <c r="Z25" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM25" s="2">
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
-      <c r="AA25" s="3">
+      <c r="AN25" s="3">
         <v>0.1159687288999377</v>
       </c>
-      <c r="AB25" s="3">
+      <c r="AO25" s="3">
         <v>0.3253760936579731</v>
       </c>
-      <c r="AE25" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR25" s="2">
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
-      <c r="AF25" s="3">
+      <c r="AS25" s="3">
         <v>8.2789932906881553E-2</v>
       </c>
-      <c r="AG25" s="3">
+      <c r="AT25" s="3">
         <v>0.22213151164887629</v>
       </c>
     </row>
-    <row r="26" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -4069,43 +4730,46 @@
         <v>22</v>
       </c>
       <c r="N26" s="3">
-        <v>0.54926529749374287</v>
+        <v>0.96837786313145813</v>
       </c>
       <c r="O26" s="3">
-        <v>0.48954710522503969</v>
-      </c>
-      <c r="U26" s="2">
-        <f t="shared" si="3"/>
+        <v>0.64759840164855664</v>
+      </c>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="AH26" s="2">
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="V26" s="3">
+      <c r="AI26" s="3">
         <v>0.94756894863843066</v>
       </c>
-      <c r="W26" s="3">
+      <c r="AJ26" s="3">
         <v>0.66667210354049744</v>
       </c>
-      <c r="Z26" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM26" s="2">
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
-      <c r="AA26" s="3">
+      <c r="AN26" s="3">
         <v>0.1188156322728026</v>
       </c>
-      <c r="AB26" s="3">
+      <c r="AO26" s="3">
         <v>0.30442573730136491</v>
       </c>
-      <c r="AE26" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR26" s="2">
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
-      <c r="AF26" s="3">
+      <c r="AS26" s="3">
         <v>8.1020708579676914E-2</v>
       </c>
-      <c r="AG26" s="3">
+      <c r="AT26" s="3">
         <v>0.21822296232072161</v>
       </c>
     </row>
-    <row r="27" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -4131,43 +4795,76 @@
         <v>23</v>
       </c>
       <c r="N27" s="3">
-        <v>0.54962587441459609</v>
+        <v>0.96880271632125947</v>
       </c>
       <c r="O27" s="3">
-        <v>0.52952299768277711</v>
-      </c>
-      <c r="U27" s="2">
-        <f t="shared" si="3"/>
+        <v>0.66406028222756097</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="R27" s="3">
+        <f>AVERAGE(R5:R24)</f>
+        <v>0.91952186662243096</v>
+      </c>
+      <c r="S27" s="3">
+        <f>AVERAGE(S5:S24)</f>
+        <v>0.65549279340980349</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="V27" s="3">
+        <f>AVERAGE(V5:V24)</f>
+        <v>1.4995960212204068E-2</v>
+      </c>
+      <c r="W27" s="3">
+        <f>AVERAGE(W5:W24)</f>
+        <v>0.10315335131989704</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z27" s="3">
+        <f>AVERAGE(Z5:Z24)</f>
+        <v>1.0121142151391774E-2</v>
+      </c>
+      <c r="AA27" s="3">
+        <f>AVERAGE(AA5:AA24)</f>
+        <v>0.10811159419403238</v>
+      </c>
+      <c r="AH27" s="2">
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
-      <c r="V27" s="3">
+      <c r="AI27" s="3">
         <v>0.94927941087257661</v>
       </c>
-      <c r="W27" s="3">
+      <c r="AJ27" s="3">
         <v>0.64131762871406184</v>
       </c>
-      <c r="Z27" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM27" s="2">
+        <f t="shared" si="7"/>
         <v>23</v>
       </c>
-      <c r="AA27" s="3">
+      <c r="AN27" s="3">
         <v>0.11645404150536651</v>
       </c>
-      <c r="AB27" s="3">
+      <c r="AO27" s="3">
         <v>0.31879587372270279</v>
       </c>
-      <c r="AE27" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR27" s="2">
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
-      <c r="AF27" s="3">
+      <c r="AS27" s="3">
         <v>8.1844616988188068E-2</v>
       </c>
-      <c r="AG27" s="3">
+      <c r="AT27" s="3">
         <v>0.22593443927629869</v>
       </c>
     </row>
-    <row r="28" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -4193,43 +4890,76 @@
         <v>24</v>
       </c>
       <c r="N28" s="3">
-        <v>0.56256994786424719</v>
+        <v>0.96649378793082474</v>
       </c>
       <c r="O28" s="3">
-        <v>0.49482280750057311</v>
-      </c>
-      <c r="U28" s="2">
-        <f t="shared" si="3"/>
+        <v>0.62467345504139926</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R28" s="3">
+        <f>_xlfn.STDEV.S(R5:R24)</f>
+        <v>1.0756227068956514E-2</v>
+      </c>
+      <c r="S28" s="3">
+        <f>_xlfn.STDEV.S(S5:S24)</f>
+        <v>3.2077340951335034E-2</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V28" s="3">
+        <f>_xlfn.STDEV.S(V5:V24)</f>
+        <v>2.2073866956576926E-4</v>
+      </c>
+      <c r="W28" s="3">
+        <f>_xlfn.STDEV.S(W5:W24)</f>
+        <v>5.116401957549685E-3</v>
+      </c>
+      <c r="Y28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z28" s="3">
+        <f>_xlfn.STDEV.S(Z5:Z24)</f>
+        <v>5.8977473093686837E-4</v>
+      </c>
+      <c r="AA28" s="3">
+        <f>_xlfn.STDEV.S(AA5:AA24)</f>
+        <v>7.6566451489672831E-3</v>
+      </c>
+      <c r="AH28" s="2">
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="V28" s="3">
+      <c r="AI28" s="3">
         <v>0.9515021068214562</v>
       </c>
-      <c r="W28" s="3">
+      <c r="AJ28" s="3">
         <v>0.63518254619664005</v>
       </c>
-      <c r="Z28" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM28" s="2">
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="AA28" s="3">
+      <c r="AN28" s="3">
         <v>0.1157431253931244</v>
       </c>
-      <c r="AB28" s="3">
+      <c r="AO28" s="3">
         <v>0.31943845407734389</v>
       </c>
-      <c r="AE28" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR28" s="2">
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="AF28" s="3">
+      <c r="AS28" s="3">
         <v>8.2173262857609272E-2</v>
       </c>
-      <c r="AG28" s="3">
+      <c r="AT28" s="3">
         <v>0.21537597522765939</v>
       </c>
     </row>
-    <row r="29" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -4255,43 +4985,46 @@
         <v>25</v>
       </c>
       <c r="N29" s="3">
-        <v>0.55872190267000232</v>
+        <v>0.96864685132448114</v>
       </c>
       <c r="O29" s="3">
-        <v>0.50745130933313165</v>
-      </c>
-      <c r="U29" s="2">
-        <f t="shared" si="3"/>
+        <v>0.60215066964549391</v>
+      </c>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="AH29" s="2">
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="V29" s="3">
+      <c r="AI29" s="3">
         <v>0.95079891183675846</v>
       </c>
-      <c r="W29" s="3">
+      <c r="AJ29" s="3">
         <v>0.62709149935300168</v>
       </c>
-      <c r="Z29" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM29" s="2">
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
-      <c r="AA29" s="3">
+      <c r="AN29" s="3">
         <v>0.11867626165435349</v>
       </c>
-      <c r="AB29" s="3">
+      <c r="AO29" s="3">
         <v>0.3004675508345675</v>
       </c>
-      <c r="AE29" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR29" s="2">
+        <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="AF29" s="3">
+      <c r="AS29" s="3">
         <v>8.3103598191252098E-2</v>
       </c>
-      <c r="AG29" s="3">
+      <c r="AT29" s="3">
         <v>0.21896354956737649</v>
       </c>
     </row>
-    <row r="30" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -4317,43 +5050,46 @@
         <v>26</v>
       </c>
       <c r="N30" s="3">
-        <v>0.58024609343143685</v>
+        <v>0.969671800776857</v>
       </c>
       <c r="O30" s="3">
-        <v>0.4549042117983535</v>
-      </c>
-      <c r="U30" s="2">
-        <f t="shared" si="3"/>
+        <v>0.65465714872092806</v>
+      </c>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="AH30" s="2">
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
-      <c r="V30" s="3">
+      <c r="AI30" s="3">
         <v>0.94856625043000042</v>
       </c>
-      <c r="W30" s="3">
+      <c r="AJ30" s="3">
         <v>0.66241752296418577</v>
       </c>
-      <c r="Z30" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM30" s="2">
+        <f t="shared" si="7"/>
         <v>26</v>
       </c>
-      <c r="AA30" s="3">
+      <c r="AN30" s="3">
         <v>0.1169732797623813</v>
       </c>
-      <c r="AB30" s="3">
+      <c r="AO30" s="3">
         <v>0.3032128295097809</v>
       </c>
-      <c r="AE30" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR30" s="2">
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
-      <c r="AF30" s="3">
+      <c r="AS30" s="3">
         <v>8.3415777895986545E-2</v>
       </c>
-      <c r="AG30" s="3">
+      <c r="AT30" s="3">
         <v>0.21674506623377729</v>
       </c>
     </row>
-    <row r="31" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -4379,43 +5115,46 @@
         <v>27</v>
       </c>
       <c r="N31" s="3">
-        <v>0.55112998792645951</v>
+        <v>0.97001840884810031</v>
       </c>
       <c r="O31" s="3">
-        <v>0.53296804194773317</v>
-      </c>
-      <c r="U31" s="2">
-        <f t="shared" si="3"/>
+        <v>0.60428224392327556</v>
+      </c>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="AH31" s="2">
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
-      <c r="V31" s="3">
+      <c r="AI31" s="3">
         <v>0.94916909696737206</v>
       </c>
-      <c r="W31" s="3">
+      <c r="AJ31" s="3">
         <v>0.64024763553481212</v>
       </c>
-      <c r="Z31" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM31" s="2">
+        <f t="shared" si="7"/>
         <v>27</v>
       </c>
-      <c r="AA31" s="3">
+      <c r="AN31" s="3">
         <v>0.1163453991392718</v>
       </c>
-      <c r="AB31" s="3">
+      <c r="AO31" s="3">
         <v>0.32424540470377</v>
       </c>
-      <c r="AE31" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR31" s="2">
+        <f t="shared" si="8"/>
         <v>27</v>
       </c>
-      <c r="AF31" s="3">
+      <c r="AS31" s="3">
         <v>8.199141602551098E-2</v>
       </c>
-      <c r="AG31" s="3">
+      <c r="AT31" s="3">
         <v>0.22104538512261029</v>
       </c>
     </row>
-    <row r="32" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -4441,43 +5180,46 @@
         <v>28</v>
       </c>
       <c r="N32" s="3">
-        <v>0.56136621315304436</v>
+        <v>0.96749575750699623</v>
       </c>
       <c r="O32" s="3">
-        <v>0.48908718548259972</v>
-      </c>
-      <c r="U32" s="2">
-        <f t="shared" si="3"/>
+        <v>0.65759979901366417</v>
+      </c>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="AH32" s="2">
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
-      <c r="V32" s="3">
+      <c r="AI32" s="3">
         <v>0.95126590667618927</v>
       </c>
-      <c r="W32" s="3">
+      <c r="AJ32" s="3">
         <v>0.63468850809580535</v>
       </c>
-      <c r="Z32" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM32" s="2">
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
-      <c r="AA32" s="3">
+      <c r="AN32" s="3">
         <v>0.11644616566050631</v>
       </c>
-      <c r="AB32" s="3">
+      <c r="AO32" s="3">
         <v>0.31759852383906773</v>
       </c>
-      <c r="AE32" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR32" s="2">
+        <f t="shared" si="8"/>
         <v>28</v>
       </c>
-      <c r="AF32" s="3">
+      <c r="AS32" s="3">
         <v>8.1993014509199463E-2</v>
       </c>
-      <c r="AG32" s="3">
+      <c r="AT32" s="3">
         <v>0.22662824984082541</v>
       </c>
     </row>
-    <row r="33" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -4503,43 +5245,46 @@
         <v>29</v>
       </c>
       <c r="N33" s="3">
-        <v>0.55816565108809524</v>
+        <v>0.96966002835021781</v>
       </c>
       <c r="O33" s="3">
-        <v>0.49587274033729639</v>
-      </c>
-      <c r="U33" s="2">
-        <f t="shared" si="3"/>
+        <v>0.62605676163174528</v>
+      </c>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="AH33" s="2">
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
-      <c r="V33" s="3">
+      <c r="AI33" s="3">
         <v>0.94801919875087393</v>
       </c>
-      <c r="W33" s="3">
+      <c r="AJ33" s="3">
         <v>0.63510125010181251</v>
       </c>
-      <c r="Z33" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM33" s="2">
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
-      <c r="AA33" s="3">
+      <c r="AN33" s="3">
         <v>0.11672428402742439</v>
       </c>
-      <c r="AB33" s="3">
+      <c r="AO33" s="3">
         <v>0.31902442548075549</v>
       </c>
-      <c r="AE33" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR33" s="2">
+        <f t="shared" si="8"/>
         <v>29</v>
       </c>
-      <c r="AF33" s="3">
+      <c r="AS33" s="3">
         <v>8.2309728202983323E-2</v>
       </c>
-      <c r="AG33" s="3">
+      <c r="AT33" s="3">
         <v>0.22590961366287871</v>
       </c>
     </row>
-    <row r="34" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -4565,43 +5310,46 @@
         <v>30</v>
       </c>
       <c r="N34" s="3">
-        <v>0.55260648880568741</v>
+        <v>0.97011070399065524</v>
       </c>
       <c r="O34" s="3">
-        <v>0.51932386991672441</v>
-      </c>
-      <c r="U34" s="2">
-        <f t="shared" si="3"/>
+        <v>0.61770117800353197</v>
+      </c>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="AH34" s="2">
+        <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="V34" s="3">
+      <c r="AI34" s="3">
         <v>0.94840673758908034</v>
       </c>
-      <c r="W34" s="3">
+      <c r="AJ34" s="3">
         <v>0.63280636724155181</v>
       </c>
-      <c r="Z34" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM34" s="2">
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
-      <c r="AA34" s="3">
+      <c r="AN34" s="3">
         <v>0.1169542614656538</v>
       </c>
-      <c r="AB34" s="3">
+      <c r="AO34" s="3">
         <v>0.32529631093429251</v>
       </c>
-      <c r="AE34" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR34" s="2">
+        <f t="shared" si="8"/>
         <v>30</v>
       </c>
-      <c r="AF34" s="3">
+      <c r="AS34" s="3">
         <v>8.1605759551974022E-2</v>
       </c>
-      <c r="AG34" s="3">
+      <c r="AT34" s="3">
         <v>0.22718560267952981</v>
       </c>
     </row>
-    <row r="35" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -4627,43 +5375,46 @@
         <v>31</v>
       </c>
       <c r="N35" s="3">
-        <v>0.55800231360741881</v>
+        <v>0.96684736221410073</v>
       </c>
       <c r="O35" s="3">
-        <v>0.48655174627056319</v>
-      </c>
-      <c r="U35" s="2">
-        <f t="shared" si="3"/>
+        <v>0.64167312986793201</v>
+      </c>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="AH35" s="2">
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
-      <c r="V35" s="3">
+      <c r="AI35" s="3">
         <v>0.94897277585487816</v>
       </c>
-      <c r="W35" s="3">
+      <c r="AJ35" s="3">
         <v>0.63271904361202025</v>
       </c>
-      <c r="Z35" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM35" s="2">
+        <f t="shared" si="7"/>
         <v>31</v>
       </c>
-      <c r="AA35" s="3">
+      <c r="AN35" s="3">
         <v>0.1171298554338379</v>
       </c>
-      <c r="AB35" s="3">
+      <c r="AO35" s="3">
         <v>0.30882175983954802</v>
       </c>
-      <c r="AE35" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR35" s="2">
+        <f t="shared" si="8"/>
         <v>31</v>
       </c>
-      <c r="AF35" s="3">
+      <c r="AS35" s="3">
         <v>8.0857996013291869E-2</v>
       </c>
-      <c r="AG35" s="3">
+      <c r="AT35" s="3">
         <v>0.23442192452121891</v>
       </c>
     </row>
-    <row r="36" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -4689,43 +5440,46 @@
         <v>32</v>
       </c>
       <c r="N36" s="3">
-        <v>0.57172497230820551</v>
+        <v>0.96719949468444144</v>
       </c>
       <c r="O36" s="3">
-        <v>0.46688614864403172</v>
-      </c>
-      <c r="U36" s="2">
-        <f t="shared" si="3"/>
+        <v>0.67839377188742023</v>
+      </c>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="AH36" s="2">
+        <f t="shared" si="6"/>
         <v>32</v>
       </c>
-      <c r="V36" s="3">
+      <c r="AI36" s="3">
         <v>0.94989485658998185</v>
       </c>
-      <c r="W36" s="3">
+      <c r="AJ36" s="3">
         <v>0.62461230834730297</v>
       </c>
-      <c r="Z36" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM36" s="2">
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
-      <c r="AA36" s="3">
+      <c r="AN36" s="3">
         <v>0.11464950412351831</v>
       </c>
-      <c r="AB36" s="3">
+      <c r="AO36" s="3">
         <v>0.31775017191690352</v>
       </c>
-      <c r="AE36" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR36" s="2">
+        <f t="shared" si="8"/>
         <v>32</v>
       </c>
-      <c r="AF36" s="3">
+      <c r="AS36" s="3">
         <v>8.268426659852357E-2</v>
       </c>
-      <c r="AG36" s="3">
+      <c r="AT36" s="3">
         <v>0.214568109380808</v>
       </c>
     </row>
-    <row r="37" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -4751,43 +5505,46 @@
         <v>33</v>
       </c>
       <c r="N37" s="3">
-        <v>0.55690763968236379</v>
+        <v>0.96705358336396263</v>
       </c>
       <c r="O37" s="3">
-        <v>0.49306054402245031</v>
-      </c>
-      <c r="U37" s="2">
-        <f t="shared" si="3"/>
+        <v>0.61966094306851316</v>
+      </c>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3"/>
+      <c r="AH37" s="2">
+        <f t="shared" si="6"/>
         <v>33</v>
       </c>
-      <c r="V37" s="3">
+      <c r="AI37" s="3">
         <v>0.94907260950292616</v>
       </c>
-      <c r="W37" s="3">
+      <c r="AJ37" s="3">
         <v>0.64995189227802974</v>
       </c>
-      <c r="Z37" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM37" s="2">
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
-      <c r="AA37" s="3">
+      <c r="AN37" s="3">
         <v>0.1192575516029472</v>
       </c>
-      <c r="AB37" s="3">
+      <c r="AO37" s="3">
         <v>0.30416485167056451</v>
       </c>
-      <c r="AE37" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR37" s="2">
+        <f t="shared" si="8"/>
         <v>33</v>
       </c>
-      <c r="AF37" s="3">
+      <c r="AS37" s="3">
         <v>8.251939102818831E-2</v>
       </c>
-      <c r="AG37" s="3">
+      <c r="AT37" s="3">
         <v>0.22075695663214909</v>
       </c>
     </row>
-    <row r="38" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -4813,43 +5570,46 @@
         <v>34</v>
       </c>
       <c r="N38" s="3">
-        <v>0.56852446262164502</v>
+        <v>0.96605608814051069</v>
       </c>
       <c r="O38" s="3">
-        <v>0.46651930880157372</v>
-      </c>
-      <c r="U38" s="2">
-        <f t="shared" si="3"/>
+        <v>0.6347610026260514</v>
+      </c>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3"/>
+      <c r="AH38" s="2">
+        <f t="shared" si="6"/>
         <v>34</v>
       </c>
-      <c r="V38" s="3">
+      <c r="AI38" s="3">
         <v>0.94705888623340939</v>
       </c>
-      <c r="W38" s="3">
+      <c r="AJ38" s="3">
         <v>0.68579049132970538</v>
       </c>
-      <c r="Z38" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM38" s="2">
+        <f t="shared" si="7"/>
         <v>34</v>
       </c>
-      <c r="AA38" s="3">
+      <c r="AN38" s="3">
         <v>0.116326574624316</v>
       </c>
-      <c r="AB38" s="3">
+      <c r="AO38" s="3">
         <v>0.31101830390379742</v>
       </c>
-      <c r="AE38" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR38" s="2">
+        <f t="shared" si="8"/>
         <v>34</v>
       </c>
-      <c r="AF38" s="3">
+      <c r="AS38" s="3">
         <v>8.2179918254379064E-2</v>
       </c>
-      <c r="AG38" s="3">
+      <c r="AT38" s="3">
         <v>0.22428725388674131</v>
       </c>
     </row>
-    <row r="39" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -4875,43 +5635,46 @@
         <v>35</v>
       </c>
       <c r="N39" s="3">
-        <v>0.56115963175501893</v>
+        <v>0.96387596753140237</v>
       </c>
       <c r="O39" s="3">
-        <v>0.48126092422625771</v>
-      </c>
-      <c r="U39" s="2">
-        <f t="shared" si="3"/>
+        <v>0.66804475102805649</v>
+      </c>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="AH39" s="2">
+        <f t="shared" si="6"/>
         <v>35</v>
       </c>
-      <c r="V39" s="3">
+      <c r="AI39" s="3">
         <v>0.94958304174087971</v>
       </c>
-      <c r="W39" s="3">
+      <c r="AJ39" s="3">
         <v>0.65048634766205182</v>
       </c>
-      <c r="Z39" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM39" s="2">
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
-      <c r="AA39" s="3">
+      <c r="AN39" s="3">
         <v>0.11657180545628169</v>
       </c>
-      <c r="AB39" s="3">
+      <c r="AO39" s="3">
         <v>0.32267682431196071</v>
       </c>
-      <c r="AE39" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR39" s="2">
+        <f t="shared" si="8"/>
         <v>35</v>
       </c>
-      <c r="AF39" s="3">
+      <c r="AS39" s="3">
         <v>8.434088398931025E-2</v>
       </c>
-      <c r="AG39" s="3">
+      <c r="AT39" s="3">
         <v>0.2074504515956096</v>
       </c>
     </row>
-    <row r="40" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -4937,43 +5700,46 @@
         <v>36</v>
       </c>
       <c r="N40" s="3">
-        <v>0.56560546594344041</v>
+        <v>0.9666570417754452</v>
       </c>
       <c r="O40" s="3">
-        <v>0.44550476415424028</v>
-      </c>
-      <c r="U40" s="2">
-        <f t="shared" si="3"/>
+        <v>0.64572779773133293</v>
+      </c>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="AH40" s="2">
+        <f t="shared" si="6"/>
         <v>36</v>
       </c>
-      <c r="V40" s="3">
+      <c r="AI40" s="3">
         <v>0.94913214919623734</v>
       </c>
-      <c r="W40" s="3">
+      <c r="AJ40" s="3">
         <v>0.65518227950724151</v>
       </c>
-      <c r="Z40" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM40" s="2">
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
-      <c r="AA40" s="3">
+      <c r="AN40" s="3">
         <v>0.1175172251952756</v>
       </c>
-      <c r="AB40" s="3">
+      <c r="AO40" s="3">
         <v>0.29687029675893889</v>
       </c>
-      <c r="AE40" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR40" s="2">
+        <f t="shared" si="8"/>
         <v>36</v>
       </c>
-      <c r="AF40" s="3">
+      <c r="AS40" s="3">
         <v>8.1053474524131197E-2</v>
       </c>
-      <c r="AG40" s="3">
+      <c r="AT40" s="3">
         <v>0.2234413775313043</v>
       </c>
     </row>
-    <row r="41" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -4999,43 +5765,46 @@
         <v>37</v>
       </c>
       <c r="N41" s="3">
-        <v>0.55963266544690693</v>
+        <v>0.96843934500342366</v>
       </c>
       <c r="O41" s="3">
-        <v>0.51037081587766808</v>
-      </c>
-      <c r="U41" s="2">
-        <f t="shared" si="3"/>
+        <v>0.69274380341907627</v>
+      </c>
+      <c r="Q41" s="2"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="AH41" s="2">
+        <f t="shared" si="6"/>
         <v>37</v>
       </c>
-      <c r="V41" s="3">
+      <c r="AI41" s="3">
         <v>0.94985408030840934</v>
       </c>
-      <c r="W41" s="3">
+      <c r="AJ41" s="3">
         <v>0.63504508315405128</v>
       </c>
-      <c r="Z41" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM41" s="2">
+        <f t="shared" si="7"/>
         <v>37</v>
       </c>
-      <c r="AA41" s="3">
+      <c r="AN41" s="3">
         <v>0.1163592268528314</v>
       </c>
-      <c r="AB41" s="3">
+      <c r="AO41" s="3">
         <v>0.33429847081729869</v>
       </c>
-      <c r="AE41" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR41" s="2">
+        <f t="shared" si="8"/>
         <v>37</v>
       </c>
-      <c r="AF41" s="3">
+      <c r="AS41" s="3">
         <v>8.2970175312972821E-2</v>
       </c>
-      <c r="AG41" s="3">
+      <c r="AT41" s="3">
         <v>0.21663735395507289</v>
       </c>
     </row>
-    <row r="42" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -5061,43 +5830,46 @@
         <v>38</v>
       </c>
       <c r="N42" s="3">
-        <v>0.56085220176285255</v>
+        <v>0.96998048909780143</v>
       </c>
       <c r="O42" s="3">
-        <v>0.47270852034382588</v>
-      </c>
-      <c r="U42" s="2">
-        <f t="shared" si="3"/>
+        <v>0.64411337815721204</v>
+      </c>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="AH42" s="2">
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
-      <c r="V42" s="3">
+      <c r="AI42" s="3">
         <v>0.94749047901522876</v>
       </c>
-      <c r="W42" s="3">
+      <c r="AJ42" s="3">
         <v>0.65365982615793783</v>
       </c>
-      <c r="Z42" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM42" s="2">
+        <f t="shared" si="7"/>
         <v>38</v>
       </c>
-      <c r="AA42" s="3">
+      <c r="AN42" s="3">
         <v>0.1171025183624865</v>
       </c>
-      <c r="AB42" s="3">
+      <c r="AO42" s="3">
         <v>0.30969333488200551</v>
       </c>
-      <c r="AE42" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR42" s="2">
+        <f t="shared" si="8"/>
         <v>38</v>
       </c>
-      <c r="AF42" s="3">
+      <c r="AS42" s="3">
         <v>8.2391958007001886E-2</v>
       </c>
-      <c r="AG42" s="3">
+      <c r="AT42" s="3">
         <v>0.2213559784908905</v>
       </c>
     </row>
-    <row r="43" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -5123,43 +5895,46 @@
         <v>39</v>
       </c>
       <c r="N43" s="3">
-        <v>0.56119179626214155</v>
+        <v>0.96805387094207784</v>
       </c>
       <c r="O43" s="3">
-        <v>0.47661244911387968</v>
-      </c>
-      <c r="U43" s="2">
-        <f t="shared" si="3"/>
+        <v>0.65494419522582414</v>
+      </c>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="AH43" s="2">
+        <f t="shared" si="6"/>
         <v>39</v>
       </c>
-      <c r="V43" s="3">
+      <c r="AI43" s="3">
         <v>0.94941351161572984</v>
       </c>
-      <c r="W43" s="3">
+      <c r="AJ43" s="3">
         <v>0.64862303322456505</v>
       </c>
-      <c r="Z43" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM43" s="2">
+        <f t="shared" si="7"/>
         <v>39</v>
       </c>
-      <c r="AA43" s="3">
+      <c r="AN43" s="3">
         <v>0.1160097829524077</v>
       </c>
-      <c r="AB43" s="3">
+      <c r="AO43" s="3">
         <v>0.31411067341506499</v>
       </c>
-      <c r="AE43" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR43" s="2">
+        <f t="shared" si="8"/>
         <v>39</v>
       </c>
-      <c r="AF43" s="3">
+      <c r="AS43" s="3">
         <v>8.22429721964546E-2</v>
       </c>
-      <c r="AG43" s="3">
+      <c r="AT43" s="3">
         <v>0.22404168224471041</v>
       </c>
     </row>
-    <row r="44" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -5185,43 +5960,46 @@
         <v>40</v>
       </c>
       <c r="N44" s="3">
-        <v>0.54892211022858839</v>
+        <v>0.9677382286555406</v>
       </c>
       <c r="O44" s="3">
-        <v>0.52029955105430714</v>
-      </c>
-      <c r="U44" s="2">
-        <f t="shared" si="3"/>
+        <v>0.64027158040545418</v>
+      </c>
+      <c r="Q44" s="2"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="AH44" s="2">
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="V44" s="3">
+      <c r="AI44" s="3">
         <v>0.94713217301416419</v>
       </c>
-      <c r="W44" s="3">
+      <c r="AJ44" s="3">
         <v>0.66737832250117057</v>
       </c>
-      <c r="Z44" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM44" s="2">
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
-      <c r="AA44" s="3">
+      <c r="AN44" s="3">
         <v>0.1169842007493667</v>
       </c>
-      <c r="AB44" s="3">
+      <c r="AO44" s="3">
         <v>0.3195361200902328</v>
       </c>
-      <c r="AE44" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR44" s="2">
+        <f t="shared" si="8"/>
         <v>40</v>
       </c>
-      <c r="AF44" s="3">
+      <c r="AS44" s="3">
         <v>8.1921480878560951E-2</v>
       </c>
-      <c r="AG44" s="3">
+      <c r="AT44" s="3">
         <v>0.22349437843421341</v>
       </c>
     </row>
-    <row r="45" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -5247,43 +6025,46 @@
         <v>41</v>
       </c>
       <c r="N45" s="3">
-        <v>0.56491109036266129</v>
+        <v>0.96704033425898828</v>
       </c>
       <c r="O45" s="3">
-        <v>0.49115575136044831</v>
-      </c>
-      <c r="U45" s="2">
-        <f t="shared" si="3"/>
+        <v>0.66115814287741448</v>
+      </c>
+      <c r="Q45" s="2"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="AH45" s="2">
+        <f t="shared" si="6"/>
         <v>41</v>
       </c>
-      <c r="V45" s="3">
+      <c r="AI45" s="3">
         <v>0.94955062022533965</v>
       </c>
-      <c r="W45" s="3">
+      <c r="AJ45" s="3">
         <v>0.66217097171706796</v>
       </c>
-      <c r="Z45" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM45" s="2">
+        <f t="shared" si="7"/>
         <v>41</v>
       </c>
-      <c r="AA45" s="3">
+      <c r="AN45" s="3">
         <v>0.1156723396802683</v>
       </c>
-      <c r="AB45" s="3">
+      <c r="AO45" s="3">
         <v>0.32980129419433779</v>
       </c>
-      <c r="AE45" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR45" s="2">
+        <f t="shared" si="8"/>
         <v>41</v>
       </c>
-      <c r="AF45" s="3">
+      <c r="AS45" s="3">
         <v>8.265138180769839E-2</v>
       </c>
-      <c r="AG45" s="3">
+      <c r="AT45" s="3">
         <v>0.2185944437724423</v>
       </c>
     </row>
-    <row r="46" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -5309,43 +6090,46 @@
         <v>42</v>
       </c>
       <c r="N46" s="3">
-        <v>0.5690967802681195</v>
+        <v>0.96756593276728253</v>
       </c>
       <c r="O46" s="3">
-        <v>0.48108643836119352</v>
-      </c>
-      <c r="U46" s="2">
-        <f t="shared" si="3"/>
+        <v>0.67334101939530366</v>
+      </c>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="AH46" s="2">
+        <f t="shared" si="6"/>
         <v>42</v>
       </c>
-      <c r="V46" s="3">
+      <c r="AI46" s="3">
         <v>0.94945515644551282</v>
       </c>
-      <c r="W46" s="3">
+      <c r="AJ46" s="3">
         <v>0.61884190231559644</v>
       </c>
-      <c r="Z46" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM46" s="2">
+        <f t="shared" si="7"/>
         <v>42</v>
       </c>
-      <c r="AA46" s="3">
+      <c r="AN46" s="3">
         <v>0.1192893179719352</v>
       </c>
-      <c r="AB46" s="3">
+      <c r="AO46" s="3">
         <v>0.30232087969819471</v>
       </c>
-      <c r="AE46" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR46" s="2">
+        <f t="shared" si="8"/>
         <v>42</v>
       </c>
-      <c r="AF46" s="3">
+      <c r="AS46" s="3">
         <v>8.1484548138303636E-2</v>
       </c>
-      <c r="AG46" s="3">
+      <c r="AT46" s="3">
         <v>0.2207778386553034</v>
       </c>
     </row>
-    <row r="47" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -5371,43 +6155,46 @@
         <v>43</v>
       </c>
       <c r="N47" s="3">
-        <v>0.55915574224950459</v>
+        <v>0.96901333066048068</v>
       </c>
       <c r="O47" s="3">
-        <v>0.49276078268304729</v>
-      </c>
-      <c r="U47" s="2">
-        <f t="shared" si="3"/>
+        <v>0.64908603701423795</v>
+      </c>
+      <c r="Q47" s="2"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="AH47" s="2">
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
-      <c r="V47" s="3">
+      <c r="AI47" s="3">
         <v>0.9495275389287956</v>
       </c>
-      <c r="W47" s="3">
+      <c r="AJ47" s="3">
         <v>0.60652038798714258</v>
       </c>
-      <c r="Z47" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM47" s="2">
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
-      <c r="AA47" s="3">
+      <c r="AN47" s="3">
         <v>0.1148393825765807</v>
       </c>
-      <c r="AB47" s="3">
+      <c r="AO47" s="3">
         <v>0.32812220282649351</v>
       </c>
-      <c r="AE47" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR47" s="2">
+        <f t="shared" si="8"/>
         <v>43</v>
       </c>
-      <c r="AF47" s="3">
+      <c r="AS47" s="3">
         <v>8.2216713090806512E-2</v>
       </c>
-      <c r="AG47" s="3">
+      <c r="AT47" s="3">
         <v>0.2176719762422053</v>
       </c>
     </row>
-    <row r="48" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -5433,43 +6220,46 @@
         <v>44</v>
       </c>
       <c r="N48" s="3">
-        <v>0.55900491735508084</v>
+        <v>0.96775676945242362</v>
       </c>
       <c r="O48" s="3">
-        <v>0.50325636406513996</v>
-      </c>
-      <c r="U48" s="2">
-        <f t="shared" si="3"/>
+        <v>0.65576711279830713</v>
+      </c>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="AH48" s="2">
+        <f t="shared" si="6"/>
         <v>44</v>
       </c>
-      <c r="V48" s="3">
+      <c r="AI48" s="3">
         <v>0.94950923407580956</v>
       </c>
-      <c r="W48" s="3">
+      <c r="AJ48" s="3">
         <v>0.64211990133419727</v>
       </c>
-      <c r="Z48" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM48" s="2">
+        <f t="shared" si="7"/>
         <v>44</v>
       </c>
-      <c r="AA48" s="3">
+      <c r="AN48" s="3">
         <v>0.1183066921327932</v>
       </c>
-      <c r="AB48" s="3">
+      <c r="AO48" s="3">
         <v>0.31167400605268719</v>
       </c>
-      <c r="AE48" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR48" s="2">
+        <f t="shared" si="8"/>
         <v>44</v>
       </c>
-      <c r="AF48" s="3">
+      <c r="AS48" s="3">
         <v>8.1229551364922783E-2</v>
       </c>
-      <c r="AG48" s="3">
+      <c r="AT48" s="3">
         <v>0.22558488513671829</v>
       </c>
     </row>
-    <row r="49" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -5495,43 +6285,46 @@
         <v>45</v>
       </c>
       <c r="N49" s="3">
-        <v>0.56987359946145311</v>
+        <v>0.96828891765935021</v>
       </c>
       <c r="O49" s="3">
-        <v>0.45790968959728179</v>
-      </c>
-      <c r="U49" s="2">
-        <f t="shared" si="3"/>
+        <v>0.67814163911810921</v>
+      </c>
+      <c r="Q49" s="2"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="AH49" s="2">
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
-      <c r="V49" s="3">
+      <c r="AI49" s="3">
         <v>0.9499083921940904</v>
       </c>
-      <c r="W49" s="3">
+      <c r="AJ49" s="3">
         <v>0.67279707299537095</v>
       </c>
-      <c r="Z49" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM49" s="2">
+        <f t="shared" si="7"/>
         <v>45</v>
       </c>
-      <c r="AA49" s="3">
+      <c r="AN49" s="3">
         <v>0.1181313888372665</v>
       </c>
-      <c r="AB49" s="3">
+      <c r="AO49" s="3">
         <v>0.2993634376661844</v>
       </c>
-      <c r="AE49" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR49" s="2">
+        <f t="shared" si="8"/>
         <v>45</v>
       </c>
-      <c r="AF49" s="3">
+      <c r="AS49" s="3">
         <v>8.1252399579726312E-2</v>
       </c>
-      <c r="AG49" s="3">
+      <c r="AT49" s="3">
         <v>0.22627686644551931</v>
       </c>
     </row>
-    <row r="50" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -5557,43 +6350,46 @@
         <v>46</v>
       </c>
       <c r="N50" s="3">
-        <v>0.57084586930465497</v>
+        <v>0.96930009417344143</v>
       </c>
       <c r="O50" s="3">
-        <v>0.44089958672100488</v>
-      </c>
-      <c r="U50" s="2">
-        <f t="shared" si="3"/>
+        <v>0.60727526617801497</v>
+      </c>
+      <c r="Q50" s="2"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="AH50" s="2">
+        <f t="shared" si="6"/>
         <v>46</v>
       </c>
-      <c r="V50" s="3">
+      <c r="AI50" s="3">
         <v>0.9486434871385766</v>
       </c>
-      <c r="W50" s="3">
+      <c r="AJ50" s="3">
         <v>0.66064148960936353</v>
       </c>
-      <c r="Z50" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM50" s="2">
+        <f t="shared" si="7"/>
         <v>46</v>
       </c>
-      <c r="AA50" s="3">
+      <c r="AN50" s="3">
         <v>0.11526373697328469</v>
       </c>
-      <c r="AB50" s="3">
+      <c r="AO50" s="3">
         <v>0.32834649138557082</v>
       </c>
-      <c r="AE50" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR50" s="2">
+        <f t="shared" si="8"/>
         <v>46</v>
       </c>
-      <c r="AF50" s="3">
+      <c r="AS50" s="3">
         <v>8.1913761806771665E-2</v>
       </c>
-      <c r="AG50" s="3">
+      <c r="AT50" s="3">
         <v>0.22526419522709509</v>
       </c>
     </row>
-    <row r="51" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -5619,43 +6415,46 @@
         <v>47</v>
       </c>
       <c r="N51" s="3">
-        <v>0.56143080886473029</v>
+        <v>0.96898516070522911</v>
       </c>
       <c r="O51" s="3">
-        <v>0.50041944569344787</v>
-      </c>
-      <c r="U51" s="2">
-        <f t="shared" si="3"/>
+        <v>0.61564138999521623</v>
+      </c>
+      <c r="Q51" s="2"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="AH51" s="2">
+        <f t="shared" si="6"/>
         <v>47</v>
       </c>
-      <c r="V51" s="3">
+      <c r="AI51" s="3">
         <v>0.95056760645959915</v>
       </c>
-      <c r="W51" s="3">
+      <c r="AJ51" s="3">
         <v>0.63749684147528407</v>
       </c>
-      <c r="Z51" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM51" s="2">
+        <f t="shared" si="7"/>
         <v>47</v>
       </c>
-      <c r="AA51" s="3">
+      <c r="AN51" s="3">
         <v>0.1167540156878106</v>
       </c>
-      <c r="AB51" s="3">
+      <c r="AO51" s="3">
         <v>0.31376120183153111</v>
       </c>
-      <c r="AE51" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR51" s="2">
+        <f t="shared" si="8"/>
         <v>47</v>
       </c>
-      <c r="AF51" s="3">
+      <c r="AS51" s="3">
         <v>8.2386580208719126E-2</v>
       </c>
-      <c r="AG51" s="3">
+      <c r="AT51" s="3">
         <v>0.2183309121651047</v>
       </c>
     </row>
-    <row r="52" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -5681,43 +6480,46 @@
         <v>48</v>
       </c>
       <c r="N52" s="3">
-        <v>0.57169128734075436</v>
+        <v>0.9691639735694535</v>
       </c>
       <c r="O52" s="3">
-        <v>0.44325058191149919</v>
-      </c>
-      <c r="U52" s="2">
-        <f t="shared" si="3"/>
+        <v>0.65324580217227091</v>
+      </c>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="AH52" s="2">
+        <f t="shared" si="6"/>
         <v>48</v>
       </c>
-      <c r="V52" s="3">
+      <c r="AI52" s="3">
         <v>0.9491752781596875</v>
       </c>
-      <c r="W52" s="3">
+      <c r="AJ52" s="3">
         <v>0.62266464437681956</v>
       </c>
-      <c r="Z52" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM52" s="2">
+        <f t="shared" si="7"/>
         <v>48</v>
       </c>
-      <c r="AA52" s="3">
+      <c r="AN52" s="3">
         <v>0.115755029130523</v>
       </c>
-      <c r="AB52" s="3">
+      <c r="AO52" s="3">
         <v>0.316101255139209</v>
       </c>
-      <c r="AE52" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR52" s="2">
+        <f t="shared" si="8"/>
         <v>48</v>
       </c>
-      <c r="AF52" s="3">
+      <c r="AS52" s="3">
         <v>8.2620642193867777E-2</v>
       </c>
-      <c r="AG52" s="3">
+      <c r="AT52" s="3">
         <v>0.2183574957645468</v>
       </c>
     </row>
-    <row r="53" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -5743,43 +6545,46 @@
         <v>49</v>
       </c>
       <c r="N53" s="3">
-        <v>0.57062196426779366</v>
+        <v>0.96380286377543911</v>
       </c>
       <c r="O53" s="3">
-        <v>0.46956736524243903</v>
-      </c>
-      <c r="U53" s="2">
-        <f t="shared" si="3"/>
+        <v>0.6283908719423843</v>
+      </c>
+      <c r="Q53" s="2"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3"/>
+      <c r="AH53" s="2">
+        <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="V53" s="3">
+      <c r="AI53" s="3">
         <v>0.95023491224099565</v>
       </c>
-      <c r="W53" s="3">
+      <c r="AJ53" s="3">
         <v>0.6234164050981541</v>
       </c>
-      <c r="Z53" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM53" s="2">
+        <f t="shared" si="7"/>
         <v>49</v>
       </c>
-      <c r="AA53" s="3">
+      <c r="AN53" s="3">
         <v>0.1179774430612817</v>
       </c>
-      <c r="AB53" s="3">
+      <c r="AO53" s="3">
         <v>0.31719008723074549</v>
       </c>
-      <c r="AE53" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR53" s="2">
+        <f t="shared" si="8"/>
         <v>49</v>
       </c>
-      <c r="AF53" s="3">
+      <c r="AS53" s="3">
         <v>8.317294504866625E-2</v>
       </c>
-      <c r="AG53" s="3">
+      <c r="AT53" s="3">
         <v>0.2208504624832697</v>
       </c>
     </row>
-    <row r="54" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -5805,43 +6610,46 @@
         <v>50</v>
       </c>
       <c r="N54" s="3">
-        <v>0.56712552347473832</v>
+        <v>0.96876204770486285</v>
       </c>
       <c r="O54" s="3">
-        <v>0.47284169948414362</v>
-      </c>
-      <c r="U54" s="2">
-        <f t="shared" si="3"/>
+        <v>0.62714655469404723</v>
+      </c>
+      <c r="Q54" s="2"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3"/>
+      <c r="AH54" s="2">
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
-      <c r="V54" s="3">
+      <c r="AI54" s="3">
         <v>0.94889179727122863</v>
       </c>
-      <c r="W54" s="3">
+      <c r="AJ54" s="3">
         <v>0.67125972957766566</v>
       </c>
-      <c r="Z54" s="2">
-        <f t="shared" si="4"/>
+      <c r="AM54" s="2">
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
-      <c r="AA54" s="3">
+      <c r="AN54" s="3">
         <v>0.11672725996177399</v>
       </c>
-      <c r="AB54" s="3">
+      <c r="AO54" s="3">
         <v>0.31912823714411509</v>
       </c>
-      <c r="AE54" s="2">
-        <f t="shared" si="5"/>
+      <c r="AR54" s="2">
+        <f t="shared" si="8"/>
         <v>50</v>
       </c>
-      <c r="AF54" s="3">
+      <c r="AS54" s="3">
         <v>8.2903110305879796E-2</v>
       </c>
-      <c r="AG54" s="3">
+      <c r="AT54" s="3">
         <v>0.22718864352021659</v>
       </c>
     </row>
-    <row r="56" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -5869,47 +6677,47 @@
       </c>
       <c r="N56" s="3">
         <f>AVERAGE(N5:N54)</f>
-        <v>0.56262746603805336</v>
+        <v>0.96761304087691868</v>
       </c>
       <c r="O56" s="3">
         <f>AVERAGE(O5:O54)</f>
-        <v>0.47880946680814424</v>
-      </c>
-      <c r="U56" s="2" t="s">
+        <v>0.64365849781482753</v>
+      </c>
+      <c r="AH56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="V56" s="3">
-        <f>AVERAGE(V5:V54)</f>
+      <c r="AI56" s="3">
+        <f>AVERAGE(AI5:AI54)</f>
         <v>0.94913546384240977</v>
       </c>
-      <c r="W56" s="3">
-        <f>AVERAGE(W5:W54)</f>
+      <c r="AJ56" s="3">
+        <f>AVERAGE(AJ5:AJ54)</f>
         <v>0.64518888293192622</v>
       </c>
-      <c r="Z56" s="2" t="s">
+      <c r="AM56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AA56" s="3">
-        <f>AVERAGE(AA5:AA54)</f>
+      <c r="AN56" s="3">
+        <f>AVERAGE(AN5:AN54)</f>
         <v>0.11699947269078689</v>
       </c>
-      <c r="AB56" s="3">
-        <f>AVERAGE(AB5:AB54)</f>
+      <c r="AO56" s="3">
+        <f>AVERAGE(AO5:AO54)</f>
         <v>0.31308656886454217</v>
       </c>
-      <c r="AE56" s="2" t="s">
+      <c r="AR56" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="AF56" s="3">
-        <f>AVERAGE(AF5:AF54)</f>
+      <c r="AS56" s="3">
+        <f>AVERAGE(AS5:AS54)</f>
         <v>8.2193910513009422E-2</v>
       </c>
-      <c r="AG56" s="3">
-        <f>AVERAGE(AG5:AG54)</f>
+      <c r="AT56" s="3">
+        <f>AVERAGE(AT5:AT54)</f>
         <v>0.22170521049141068</v>
       </c>
     </row>
-    <row r="57" spans="3:33" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:46" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -5937,43 +6745,43 @@
       </c>
       <c r="N57" s="3">
         <f>_xlfn.STDEV.S(N5:N54)</f>
-        <v>7.4995626254446349E-3</v>
+        <v>1.6013737950829094E-3</v>
       </c>
       <c r="O57" s="3">
         <f>_xlfn.STDEV.S(O5:O54)</f>
-        <v>2.6543667788147089E-2</v>
-      </c>
-      <c r="U57" s="2" t="s">
+        <v>2.280233943453298E-2</v>
+      </c>
+      <c r="AH57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="V57" s="3">
-        <f>_xlfn.STDEV.S(V5:V54)</f>
+      <c r="AI57" s="3">
+        <f>_xlfn.STDEV.S(AI5:AI54)</f>
         <v>1.0061875462076956E-3</v>
       </c>
-      <c r="W57" s="3">
-        <f>_xlfn.STDEV.S(W5:W54)</f>
+      <c r="AJ57" s="3">
+        <f>_xlfn.STDEV.S(AJ5:AJ54)</f>
         <v>2.0441479091949693E-2</v>
       </c>
-      <c r="Z57" s="2" t="s">
+      <c r="AM57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AA57" s="3">
-        <f>_xlfn.STDEV.S(AA5:AA54)</f>
+      <c r="AN57" s="3">
+        <f>_xlfn.STDEV.S(AN5:AN54)</f>
         <v>1.0573885580347465E-3</v>
       </c>
-      <c r="AB57" s="3">
-        <f>_xlfn.STDEV.S(AB5:AB54)</f>
+      <c r="AO57" s="3">
+        <f>_xlfn.STDEV.S(AO5:AO54)</f>
         <v>9.2969639757002707E-3</v>
       </c>
-      <c r="AE57" s="2" t="s">
+      <c r="AR57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="AF57" s="3">
-        <f>_xlfn.STDEV.S(AF5:AF54)</f>
+      <c r="AS57" s="3">
+        <f>_xlfn.STDEV.S(AS5:AS54)</f>
         <v>6.7919170904217252E-4</v>
       </c>
-      <c r="AG57" s="3">
-        <f>_xlfn.STDEV.S(AG5:AG54)</f>
+      <c r="AT57" s="3">
+        <f>_xlfn.STDEV.S(AT5:AT54)</f>
         <v>5.2278534035366938E-3</v>
       </c>
     </row>
@@ -5987,7 +6795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>

</xml_diff>